<commit_message>
add fetch link info
</commit_message>
<xml_diff>
--- a/harvest/tencent/青蜂侠-阅读量数据统计.xlsx
+++ b/harvest/tencent/青蜂侠-阅读量数据统计.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C164"/>
+  <dimension ref="A1:C328"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -393,1800 +393,3604 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>湖北省省长王晓东：对肺炎疫情感到痛心、内疚、自责</v>
+        <v>武汉方舱医院“KTV”开唱啦！医护人员唱歌患者伴舞</v>
       </c>
       <c r="B2">
-        <v>179161</v>
+        <v>362974</v>
       </c>
       <c r="C2" t="str">
-        <v>2020-01-26 23:43</v>
+        <v>2020-02-16 22:53</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>摄影师航拍镜头下武汉的一天：我从未见过这样的武汉</v>
+        <v>男子违规出小区被拦 恼羞成怒后竟对录像女子拳打脚踢</v>
       </c>
       <c r="B3">
-        <v>4275185</v>
+        <v>179625</v>
       </c>
       <c r="C3" t="str">
-        <v>2020-01-26 23:43</v>
+        <v>2020-02-16 21:55</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>武汉市长戴口罩出席肺炎新闻发布会：确诊病例或再增加1千例左右</v>
+        <v>疫情当前日本多地举办马拉松！近10万人参赛 有选手戴口罩跑步</v>
       </c>
       <c r="B4">
-        <v>2468567</v>
+        <v>673005</v>
       </c>
       <c r="C4" t="str">
-        <v>2020-01-26 22:49</v>
+        <v>2020-02-16 21:44</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>新型肺炎患者确诊前坐遍青岛所有地铁 官方：所乘线路没有绕行</v>
+        <v>疫情期间男子售卖假口罩！民警怒吼：你的良心痛不痛？</v>
       </c>
       <c r="B5">
-        <v>23864</v>
+        <v>214972</v>
       </c>
       <c r="C5" t="str">
-        <v>2020-01-26 21:50</v>
+        <v>2020-02-16 21:39</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>航拍：武汉雷神山医院开建 场地平整工作已经全面启动</v>
+        <v>防护服里“憋”太久，执勤民警跳“大风车” 旁边两同事傻眼了…</v>
       </c>
       <c r="B6">
-        <v>11007</v>
+        <v>106475</v>
       </c>
       <c r="C6" t="str">
-        <v>2020-01-26 21:49</v>
+        <v>2020-02-16 21:28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>春节假期延长首座城市出炉 国家卫健委专家提议：居家隔离</v>
+        <v>待春暖花开，欢送二老出院！这对耄耋夫妻的爱情令火神山医护动容</v>
       </c>
       <c r="B7">
-        <v>19786</v>
+        <v>289402</v>
       </c>
       <c r="C7" t="str">
-        <v>2020-01-26 20:11</v>
+        <v>2020-02-16 20:17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>中国疾控中心主任：我拍着胸口讲，疫苗肯定会研发成功</v>
+        <v>疫情中的爱情：夫妻抗疫20多天首次相遇，20秒后他却驾车离去</v>
       </c>
       <c r="B8">
-        <v>91565</v>
+        <v>64538</v>
       </c>
       <c r="C8" t="str">
-        <v>2020-01-26 19:20</v>
+        <v>2020-02-16 20:02</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>官方是否瞒报实际患病人数？卫健委：所有信息均已公示</v>
+        <v>武汉雷神山医院院长：疫情的拐点已经来到 我很有信心</v>
       </c>
       <c r="B9">
-        <v>37697</v>
+        <v>97297</v>
       </c>
       <c r="C9" t="str">
-        <v>2020-01-26 19:02</v>
+        <v>2020-02-16 19:16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>中国疾控中心主任：相信谣言选择恐慌，所造损失会比疫情更大</v>
+        <v>当发射火箭的手开始扛水泥！网友：向中国军人致敬！</v>
       </c>
       <c r="B10">
-        <v>22254</v>
+        <v>6458</v>
       </c>
       <c r="C10" t="str">
-        <v>2020-01-26 18:19</v>
+        <v>2020-02-16 18:34</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>武汉记者街头直播数度哽咽：我的武汉一定会好起来！</v>
+        <v>北京一患者回京未隔离14天 致单位几十人被隔离</v>
       </c>
       <c r="B11">
-        <v>1182338</v>
+        <v>219353</v>
       </c>
       <c r="C11" t="str">
-        <v>2020-01-26 16:41</v>
+        <v>2020-02-16 18:11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>国家卫健委：病毒传播力似乎有所增强，疫情进入比较严重复杂时期</v>
+        <v>疾控中心专家：空气净化器不一定能过滤病毒</v>
       </c>
       <c r="B12">
-        <v>1708995</v>
+        <v>17621</v>
       </c>
       <c r="C12" t="str">
-        <v>2020-01-26 16:18</v>
+        <v>2020-02-16 17:42</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>国家卫健委：春节一周假期是大隔离大消毒最佳窗ロ期</v>
+        <v>广东3名康复者捐献血浆：国家救了我 我也要救回更多的人</v>
       </c>
       <c r="B13">
-        <v>253263</v>
+        <v>185250</v>
       </c>
       <c r="C13" t="str">
-        <v>2020-01-26 16:05</v>
+        <v>2020-02-16 17:40</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>卫健委：今明将再派1600人的医疗队驰援武汉 还有上千人随时待命</v>
+        <v>湖北宜昌市长：疫情依然严峻复杂，重症、危重症较多</v>
       </c>
       <c r="B14">
-        <v>2955103</v>
+        <v>19964</v>
       </c>
       <c r="C14" t="str">
-        <v>2020-01-26 16:04</v>
+        <v>2020-02-16 17:37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>一句“我爱你”让人泪奔！河南医疗队驰援武汉 丈夫送妻失声掩面</v>
+        <v>大学生在战“疫”！10所高校400多人自发网上辅导一线医护子女功课</v>
       </c>
       <c r="B15">
-        <v>3737370</v>
+        <v>103011</v>
       </c>
       <c r="C15" t="str">
-        <v>2020-01-26 15:04</v>
+        <v>2020-02-16 17:33</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>分秒必争！震撼航拍：武汉火神山医院三天施工实况</v>
+        <v>视频版来了！兰州拉面馆一人一桌塑料布隔离 网友：吃出考场仪式感</v>
       </c>
       <c r="B16">
-        <v>95517</v>
+        <v>96769</v>
       </c>
       <c r="C16" t="str">
-        <v>2020-01-26 15:00</v>
+        <v>2020-02-16 17:31</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>传染病专家桂希恩：预计正月十五前武汉市疫情可能出现“拐点”</v>
+        <v>志愿者街头值守随手机音乐“蹦迪” 市民：疫情过后一起去！</v>
       </c>
       <c r="B17">
-        <v>916123</v>
+        <v>871312</v>
       </c>
       <c r="C17" t="str">
-        <v>2020-01-26 14:47</v>
+        <v>2020-02-16 17:30</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>女子与武汉好友在拉萨逛街 还拍视频妄称“不怕病毒” 目前已被防控</v>
+        <v>国家卫健委：不应限制医护、公安等外出工作人员返回小区</v>
       </c>
       <c r="B18">
-        <v>997918</v>
+        <v>2742689</v>
       </c>
       <c r="C18" t="str">
-        <v>2020-01-26 14:26</v>
+        <v>2020-02-16 17:22</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>“爸爸你会不会死”刚返乡就去支援武汉，儿子一句话让他忍不住流泪</v>
+        <v>从外面回家鞋子需要消毒吗？怎么消毒？中国疾控中心专家回应</v>
       </c>
       <c r="B19">
-        <v>1502568</v>
+        <v>650965</v>
       </c>
       <c r="C19" t="str">
-        <v>2020-01-26 09:38</v>
+        <v>2020-02-16 17:07</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>抗疫一线医生的一封家书：对不起儿子，妈妈没有听你的话</v>
+        <v>北京疾控发布2月15日新冠肺炎新发病例活动小区或场所</v>
       </c>
       <c r="B20">
-        <v>260888</v>
+        <v>11520</v>
       </c>
       <c r="C20" t="str">
-        <v>2020-01-26 09:36</v>
+        <v>2020-02-16 16:41</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>女护士除夕夜剪去长发支援武汉 网友：你们永远是最美的白衣天使</v>
+        <v>红外热成像体温仪能否测温准确？专家：精确性会受环境因素影响</v>
       </c>
       <c r="B21">
-        <v>11946</v>
+        <v>46139</v>
       </c>
       <c r="C21" t="str">
-        <v>2020-01-26 09:30</v>
+        <v>2020-02-16 16:35</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>全国确诊新型肺炎1975例 医生家庭演示如何进行抗疫防护措施</v>
+        <v>什么样的地方可以作为集中隔离观察点？中疾控专家回应</v>
       </c>
       <c r="B22">
-        <v>130239</v>
+        <v>71777</v>
       </c>
       <c r="C22" t="str">
-        <v>2020-01-26 09:17</v>
+        <v>2020-02-16 16:23</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>128名火神山医院建设工人组建党员突击队</v>
+        <v>中疾控专家：在不具备条件的地区，特殊人群密切接触者可居家观察</v>
       </c>
       <c r="B23">
-        <v>18391</v>
+        <v>43490</v>
       </c>
       <c r="C23" t="str">
-        <v>2020-01-26 08:26</v>
+        <v>2020-02-16 16:17</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>硬核！东莞建筑群集体亮灯 滚动劝市民宅在家：答应我，做健康小胖</v>
+        <v>国家卫健委回应基层防疫人员负担重：让大家的时间花在刀刃上</v>
       </c>
       <c r="B24">
-        <v>2701985</v>
+        <v>1459</v>
       </c>
       <c r="C24" t="str">
-        <v>2020-01-26 08:12</v>
+        <v>2020-02-16 16:15</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>湖北黄冈48小时改建黄冈版“小汤山”医院  1月27日投入使用！</v>
+        <v>中疾控专家：不应把全小区都作为密切接触者 需经过综合判定</v>
       </c>
       <c r="B25">
-        <v>34980</v>
+        <v>2753</v>
       </c>
       <c r="C25" t="str">
-        <v>2020-01-26 08:02</v>
+        <v>2020-02-16 16:13</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>UP主实拍武汉街头：即使城市封闭，我们也不是一座孤岛</v>
+        <v>志愿者街头值守随手机音乐“蹦迪” 市民：疫情过后一起去蹦迪！</v>
       </c>
       <c r="B26">
-        <v>1708331</v>
+        <v>131</v>
       </c>
       <c r="C26" t="str">
-        <v>2020-01-26 07:59</v>
+        <v>2020-02-16 15:52</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>中央对防疫工作再部署：战胜恐惧是战胜疫情的第一步</v>
+        <v>全国各地疫情防控效果显现：重症占确诊病例比例明显下降</v>
       </c>
       <c r="B27">
-        <v>6206</v>
+        <v>34144</v>
       </c>
       <c r="C27" t="str">
-        <v>2020-01-26 07:48</v>
+        <v>2020-02-16 15:49</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>留守家长的“心酸”，见面2分钟只为送顿“年夜饭”</v>
+        <v>想让他们吃口热饭，大爷挑扁担步行十几里给防疫人员送微波炉</v>
       </c>
       <c r="B28">
-        <v>6096</v>
+        <v>50984</v>
       </c>
       <c r="C28" t="str">
-        <v>2020-01-26 00:19</v>
+        <v>2020-02-16 15:33</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>搞笑又心酸！武汉人夜晚隔空喊话：“对面的，吵下架，要疯鸟”</v>
+        <v>女子隔离期外出醉酒不戴口罩殴打门卫被刑拘 酒醒后发现走错小区了</v>
       </c>
       <c r="B29">
-        <v>6276958</v>
+        <v>56251</v>
       </c>
       <c r="C29" t="str">
-        <v>2020-01-25 23:59</v>
+        <v>2020-02-16 15:27</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>为什么武汉要实施进出人员管控？传染病学专家：疫情已经刻不容缓</v>
+        <v>双胞胎护士姐妹花双双推迟婚期驰援襄阳：保护好自己，这战疫必胜</v>
       </c>
       <c r="B30">
-        <v>254213</v>
+        <v>40574</v>
       </c>
       <c r="C30" t="str">
-        <v>2020-01-25 22:39</v>
+        <v>2020-02-16 15:16</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>护士高速回医院上班被阻发视频求助 路遇市长安排警车护行！</v>
+        <v>硬核设卡！ 新疆哈萨克族民警防疫点弹起心爱的冬不拉</v>
       </c>
       <c r="B31">
-        <v>1210302</v>
+        <v>115697</v>
       </c>
       <c r="C31" t="str">
-        <v>2020-01-25 22:08</v>
+        <v>2020-02-16 14:57</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>“麻将馆马上给我关门！”各地农村疫情防控广播大合集 个个硬核</v>
+        <v>暖心！巴萨赛前为中国抗疫声援：同心战疫，命运与共！</v>
       </c>
       <c r="B32">
-        <v>1307407</v>
+        <v>130168</v>
       </c>
       <c r="C32" t="str">
-        <v>2020-01-25 22:04</v>
+        <v>2020-02-16 12:51</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>仅在家待了4小时，接到支援武汉的电话 丈夫义无反顾送妻出征</v>
+        <v>患者们刚跳完广场舞，武汉方舱医院的广播体操又安排上了！</v>
       </c>
       <c r="B33">
-        <v>52019</v>
+        <v>449113</v>
       </c>
       <c r="C33" t="str">
-        <v>2020-01-25 20:58</v>
+        <v>2020-02-16 12:49</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>硬核河南又来了！15辆婚庆礼炮车变宣传车 循环广播防疫知识</v>
+        <v>战疫必胜!三支医疗队会师武汉，机场偶遇互喊“加油”</v>
       </c>
       <c r="B34">
-        <v>96433</v>
+        <v>160717</v>
       </c>
       <c r="C34" t="str">
-        <v>2020-01-25 19:04</v>
+        <v>2020-02-16 12:22</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>武汉多家酒店民宿自发支援医护：希望你们好好吃饭、好好睡觉！</v>
+        <v>美防长造谣抹黑重提“中国威胁论” 王毅当场回怼：全是谎言</v>
       </c>
       <c r="B35">
-        <v>13678</v>
+        <v>323372</v>
       </c>
       <c r="C35" t="str">
-        <v>2020-01-25 18:00</v>
+        <v>2020-02-16 11:33</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>三天捐出百万只口罩、三人带动上百人 担当的武汉年轻人！</v>
+        <v>万众一心战疫情！中国女排为武汉加油：一定能赢得这场防疫狙击战</v>
       </c>
       <c r="B36">
-        <v>53846</v>
+        <v>1528568</v>
       </c>
       <c r="C36" t="str">
-        <v>2020-01-25 16:31</v>
+        <v>2020-02-16 10:49</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>钟南山院士被传染？其所在实验室回应：谣言！</v>
+        <v>日本：新冠肺炎已开始在日本流行 新确诊病例与中国无直接关系</v>
       </c>
       <c r="B37">
-        <v>225030</v>
+        <v>1268770</v>
       </c>
       <c r="C37" t="str">
-        <v>2020-01-25 15:12</v>
+        <v>2020-02-16 09:53</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>武汉大学中南医院护士放弃与家人过年 重返抗击疫情一线：不做逃兵</v>
+        <v>守护神！门卫大爷坚守防疫岗淋成雪人 社区送来门卫房和保暖用品</v>
       </c>
       <c r="B38">
-        <v>220721</v>
+        <v>3653</v>
       </c>
       <c r="C38" t="str">
-        <v>2020-01-25 14:37</v>
+        <v>2020-02-16 09:37</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>新年快乐！感谢你们的逆向而行带来生的希望</v>
+        <v>美国驻伊拉克大使馆遭多枚火箭弹袭击 现场黑烟滚滚传出爆炸声</v>
       </c>
       <c r="B39">
-        <v>21103</v>
+        <v>4982645</v>
       </c>
       <c r="C39" t="str">
-        <v>2020-01-25 14:32</v>
+        <v>2020-02-16 09:29</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>“加油！”疫情突袭，夫妻二人双双退票坚守一线，吃饭间隙相互鼓劲</v>
+        <v>泪目！患者紧握医生双手，哽咽致谢：我看不到你的脸，但我感谢你！</v>
       </c>
       <c r="B40">
-        <v>8478</v>
+        <v>614884</v>
       </c>
       <c r="C40" t="str">
-        <v>2020-01-25 13:32</v>
+        <v>2020-02-16 09:08</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>新加坡航班载116名武汉客人抵杭州：2人发热，乘客全部被隔离</v>
+        <v>世卫总干事：中国抗击新冠肺炎疫情损失巨大，但为世界争取了时间</v>
       </c>
       <c r="B41">
-        <v>54311</v>
+        <v>119573</v>
       </c>
       <c r="C41" t="str">
-        <v>2020-01-25 11:19</v>
+        <v>2020-02-16 09:06</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>“加油！”疫情突袭，夫妻二人双双退票坚守一线，吃饭间隙相互鼓劲</v>
+        <v>“新的，快戴上”男童与家人走散 民警贴心为其戴上口罩送其返家</v>
       </c>
       <c r="B42">
-        <v>24384</v>
+        <v>4431</v>
       </c>
       <c r="C42" t="str">
-        <v>2020-01-25 11:04</v>
+        <v>2020-02-16 08:38</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>湖北多地防控物资告急！爱心企业向荆门捐赠10万只口罩解燃眉之急</v>
+        <v>嚣张男子吐口水硬闯小区脚踹工作人员 结果被老婆当街管教一顿暴揍</v>
       </c>
       <c r="B43">
-        <v>15368</v>
+        <v>3122640</v>
       </c>
       <c r="C43" t="str">
-        <v>2020-01-25 09:30</v>
+        <v>2020-02-16 08:37</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>吸烟、放鞭炮能预防新型冠状病毒性肺炎?这些谣言不能信！</v>
+        <v>这才是教育的本质和追求！河南省教育厅厅长这段话引网友共鸣</v>
       </c>
       <c r="B44">
-        <v>44032</v>
+        <v>64227</v>
       </c>
       <c r="C44" t="str">
-        <v>2020-01-25 09:26</v>
+        <v>2020-02-16 07:30</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>全国确诊1287例新型肺炎病例：军医驰援武汉，火神山医院连夜施工</v>
+        <v>嚣张男阻拦民警疫情排查，还辱骂挑衅 被抓后忏悔：我年少轻狂</v>
       </c>
       <c r="B45">
-        <v>1692688</v>
+        <v>114315</v>
       </c>
       <c r="C45" t="str">
-        <v>2020-01-25 09:03</v>
+        <v>2020-02-16 07:28</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>致敬除夕夜的“逆行者”！春晚刚开始火警警铃响起 他们飞奔下楼…</v>
+        <v>刑侦民警送别驰援一线的医护妻子 两人隔窗互伸大拇指鼓励对方</v>
       </c>
       <c r="B46">
-        <v>8986</v>
+        <v>793831</v>
       </c>
       <c r="C46" t="str">
-        <v>2020-01-25 08:53</v>
+        <v>2020-02-16 07:27</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>口罩厂加急生产画面曝光：工人3倍工资复工复产 日产24万只口罩</v>
+        <v>四川自贡荣县发生4.4级地震 当地居民：房屋左右摇晃了十几秒</v>
       </c>
       <c r="B47">
-        <v>209960</v>
+        <v>420234</v>
       </c>
       <c r="C47" t="str">
-        <v>2020-01-25 08:29</v>
+        <v>2020-02-16 07:26</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>普京为仪仗队员捡起掉落的帽子 此举引阿拉伯人狂赞：感谢尊重！</v>
+        <v>为防止人群聚集感染 湖北黄石民警号召居民：上交麻将奖口罩</v>
       </c>
       <c r="B48">
-        <v>433097</v>
+        <v>707010</v>
       </c>
       <c r="C48" t="str">
-        <v>2020-01-25 08:13</v>
+        <v>2020-02-16 06:16</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>太给力了！除夕夜空军3架运输机飞抵武汉 空军医疗队紧急驰援！</v>
+        <v>央视主播：吃劲时该加劲不能松劲 绝对不能大意失荆州</v>
       </c>
       <c r="B49">
-        <v>1770055</v>
+        <v>4408</v>
       </c>
       <c r="C49" t="str">
-        <v>2020-01-25 08:07</v>
+        <v>2020-02-16 00:49</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>“姥爷不要我了”！史上最尬拜年：别进来，赶紧走，给红包靠空投！</v>
+        <v>疫情期间男子售卖假口罩！民警怒吼：你的良心痛不痛？</v>
       </c>
       <c r="B50">
-        <v>6674629</v>
+        <v>310751</v>
       </c>
       <c r="C50" t="str">
-        <v>2020-01-25 07:35</v>
+        <v>2020-02-15 22:56</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>感染病毒的一线医生：等我脱离隔离期，一定重返战场！</v>
+        <v>心疼！火神山医院ICU护士缺氧想吐时深吸一口气 然后继续工作</v>
       </c>
       <c r="B51">
-        <v>163865</v>
+        <v>28290</v>
       </c>
       <c r="C51" t="str">
-        <v>2020-01-25 07:33</v>
+        <v>2020-02-15 22:50</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>武汉火神山医院除夕夜施工现场：与时间赛跑，致敬建设者！</v>
+        <v>无脑！无聊！美国两男子地铁恶作剧 倾倒“新冠病毒”吓坏乘客</v>
       </c>
       <c r="B52">
-        <v>433155</v>
+        <v>169234</v>
       </c>
       <c r="C52" t="str">
-        <v>2020-01-25 07:29</v>
+        <v>2020-02-15 22:26</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>致敬逆行者！各地医生除夕夜出发驰援湖北：武汉别怕，我们来了！</v>
+        <v>美媒尖锐追问湖北为何换帅 中国驻美大使这样回应</v>
       </c>
       <c r="B53">
-        <v>326743</v>
+        <v>47569</v>
       </c>
       <c r="C53" t="str">
-        <v>2020-01-25 07:20</v>
+        <v>2020-02-15 22:22</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>六大央视主播集体拜年：特别要给武汉的朋友拜年 胜利定属于大家！</v>
+        <v>现在！武汉客厅方舱医院开启KTV模式 新疆兵团医生唱《鸿雁》</v>
       </c>
       <c r="B54">
-        <v>331175</v>
+        <v>450992</v>
       </c>
       <c r="C54" t="str">
-        <v>2020-01-25 07:06</v>
+        <v>2020-02-15 20:45</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>唯一没有彩排过的春晚节目后 央视主播轮番上阵嘱咐网友：护好自己</v>
+        <v>武汉大雪，患者自拍方舱医院居住现状：暖气、电热毯、棉袄齐全</v>
       </c>
       <c r="B55">
-        <v>21901</v>
+        <v>683157</v>
       </c>
       <c r="C55" t="str">
-        <v>2020-01-25 03:26</v>
+        <v>2020-02-15 20:25</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>春晚现场致敬一线医务人员：我们在过年，你们却在帮我们过关</v>
+        <v>恭喜！武昌方舱医院12名患者顺利“出舱” 出院证明原来长这样</v>
       </c>
       <c r="B56">
-        <v>41340</v>
+        <v>2945</v>
       </c>
       <c r="C56" t="str">
-        <v>2020-01-25 00:52</v>
+        <v>2020-02-15 20:16</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>解放军来了！150名解放军医护人员包机飞武汉：交任务就是交信任</v>
+        <v>男子不戴口罩殴打民警入刑10个月 自称：因家庭矛盾喝醉了</v>
       </c>
       <c r="B57">
-        <v>33201729</v>
+        <v>6835</v>
       </c>
       <c r="C57" t="str">
-        <v>2020-01-24 23:53</v>
+        <v>2020-02-15 19:37</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>武汉抗疫一线医护人员除夕夜吐露心声 年夜饭“盒饭配酸奶”</v>
+        <v>揭秘抗疫战场上的勤务兵：不戴口罩不穿防护服，送餐送药不喊累</v>
       </c>
       <c r="B58">
-        <v>4151896</v>
+        <v>7530</v>
       </c>
       <c r="C58" t="str">
-        <v>2020-01-24 23:29</v>
+        <v>2020-02-15 19:33</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
-        <v>武汉产妇疑染新型肺炎 《生门》主治医师与死神较量保母女平安</v>
+        <v>湖北孝感62岁治愈者：严重时曾想 如果治不好就把药留给年轻人</v>
       </c>
       <c r="B59">
-        <v>147524</v>
+        <v>6595</v>
       </c>
       <c r="C59" t="str">
-        <v>2020-01-24 23:08</v>
+        <v>2020-02-15 19:32</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
-        <v>武汉“小汤山”连夜施工 工人夜色中站路边盒饭当年夜饭</v>
+        <v>做好防护！确诊小伙自述：为什么我的40多位密切接触者均未被感染</v>
       </c>
       <c r="B60">
-        <v>73295</v>
+        <v>820149</v>
       </c>
       <c r="C60" t="str">
-        <v>2020-01-24 22:19</v>
+        <v>2020-02-15 18:26</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
-        <v>除夕夜，南方医院“抗击非典零感染团队”驰援武汉！</v>
+        <v>男子隐瞒病情吐口水致2名医护人员感染：治愈即被警方带走</v>
       </c>
       <c r="B61">
-        <v>428667</v>
+        <v>566077</v>
       </c>
       <c r="C61" t="str">
-        <v>2020-01-24 22:03</v>
+        <v>2020-02-15 18:09</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
-        <v>武汉4000名车主自愿做志愿者送物资、接送医护人员上下班</v>
+        <v>科技部：加强对实验室特别是对病毒的管理，确保生物安全</v>
       </c>
       <c r="B62">
-        <v>19359</v>
+        <v>3027058</v>
       </c>
       <c r="C62" t="str">
-        <v>2020-01-24 20:46</v>
+        <v>2020-02-15 17:49</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
-        <v>“这是分内之事、责无旁贷！”原小汤山医疗队回应“千人请战书”</v>
+        <v>中疾控研究员：复工企业要对来自疫区的员工进行特别“跟踪”</v>
       </c>
       <c r="B63">
-        <v>838510</v>
+        <v>4949</v>
       </c>
       <c r="C63" t="str">
-        <v>2020-01-24 17:57</v>
+        <v>2020-02-15 17:22</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
-        <v>一份来自武汉隔离区医护人员的拜年祝福：有我们在，大家安心过年</v>
+        <v>科技部：初步排除病毒来源于已知家禽家畜 蝙蝠是最可能源头</v>
       </c>
       <c r="B64">
-        <v>88991</v>
+        <v>172082</v>
       </c>
       <c r="C64" t="str">
-        <v>2020-01-24 15:37</v>
+        <v>2020-02-15 17:19</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
-        <v>好消息！今天，武汉一疑似新型冠状病毒感染的肺炎患者出院！</v>
+        <v>中科院院士：如何抑制炎症因子风暴是治疗焦点</v>
       </c>
       <c r="B65">
-        <v>126250</v>
+        <v>117412</v>
       </c>
       <c r="C65" t="str">
-        <v>2020-01-24 14:34</v>
+        <v>2020-02-15 16:55</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
-        <v>武汉知音湖：援建“小汤山”医院工程车排起长龙 警方全力护航</v>
+        <v>科技部：瑞德西韦正在进行临床试验，期待早日得到结果</v>
       </c>
       <c r="B66">
-        <v>185008</v>
+        <v>3374</v>
       </c>
       <c r="C66" t="str">
-        <v>2020-01-24 14:34</v>
+        <v>2020-02-15 16:53</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
-        <v>驻港部队演练刺杀操向全国人民拜年：鼠年“鼠”你美</v>
+        <v>科技部：新冠肺炎部分治疗药物已初步显示出良好临床疗效</v>
       </c>
       <c r="B67">
-        <v>52327</v>
+        <v>108356</v>
       </c>
       <c r="C67" t="str">
-        <v>2020-01-24 13:38</v>
+        <v>2020-02-15 16:18</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
-        <v>现场：武汉版“小汤山”医院已开建，上百台机械同时开挖</v>
+        <v>民航局：组织9架次包机接回海外滞留湖北籍旅客1185人</v>
       </c>
       <c r="B68">
-        <v>307464</v>
+        <v>120233</v>
       </c>
       <c r="C68" t="str">
-        <v>2020-01-24 11:33</v>
+        <v>2020-02-15 16:15</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
-        <v>湖北省发布预防新型冠状病毒肺炎的中药药方</v>
+        <v>国铁集团：全国退票1.15亿张，铁路不会形成返程高峰</v>
       </c>
       <c r="B69">
-        <v>1515277</v>
+        <v>4674</v>
       </c>
       <c r="C69" t="str">
-        <v>2020-01-24 11:29</v>
+        <v>2020-02-15 15:33</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
-        <v>澳大利亚驻华大使送上新春祝福：携手共同努力 各种灾难都能被克服</v>
+        <v>国铁集团：铁路部门已下交发热旅客596人，呼吁返程旅客戴口罩少走动</v>
       </c>
       <c r="B70">
-        <v>4348</v>
+        <v>17742</v>
       </c>
       <c r="C70" t="str">
-        <v>2020-01-24 09:14</v>
+        <v>2020-02-15 15:32</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
-        <v>“懒得理你”！查尔斯王子在与各国政要握手时 跳过彭斯直接无视</v>
+        <v>交通部副部长：今年春运返程不会出现传统意义上的高峰</v>
       </c>
       <c r="B71">
-        <v>304645</v>
+        <v>6909</v>
       </c>
       <c r="C71" t="str">
-        <v>2020-01-24 09:08</v>
+        <v>2020-02-15 15:28</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
-        <v>致敬国土的守护者！王继才烈士遗孀开山岛升起五星红旗</v>
+        <v>列车上发现发热者怎么办？国铁集团：已预留席位作为临时隔离区</v>
       </c>
       <c r="B72">
-        <v>5559</v>
+        <v>191312</v>
       </c>
       <c r="C72" t="str">
-        <v>2020-01-24 09:04</v>
+        <v>2020-02-15 15:18</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
-        <v>各地医生驰援湖北 致敬最美逆行者！</v>
+        <v>民航局：截至目前民航共退票超2000万张、票面金额超200亿元</v>
       </c>
       <c r="B73">
-        <v>62035</v>
+        <v>3548</v>
       </c>
       <c r="C73" t="str">
-        <v>2020-01-24 08:57</v>
+        <v>2020-02-15 15:11</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
-        <v>国产彩虹无人机实弹打靶画面曝光 秒中靶心小车成废铁</v>
+        <v>交通运输部：今年春运客流量预计同比下降45%，无传统意义返程高峰</v>
       </c>
       <c r="B74">
-        <v>24439</v>
+        <v>2977</v>
       </c>
       <c r="C74" t="str">
-        <v>2020-01-24 08:56</v>
+        <v>2020-02-15 15:10</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
-        <v>面对疫情众志成城：武汉并非“封城”  疫情面前没有差别对待</v>
+        <v>张家界疾控中心一科长临阵脱逃 举家赴泰国避疫情被撤职</v>
       </c>
       <c r="B75">
-        <v>35937</v>
+        <v>107547</v>
       </c>
       <c r="C75" t="str">
-        <v>2020-01-24 08:54</v>
+        <v>2020-02-15 14:40</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
-        <v>硬核拜年!12国大使飙中文送祝福，春节越来越有“国际范儿” ！</v>
+        <v>什么也阻止不了我学习！方舱医院里的这股“清流”让人动容</v>
       </c>
       <c r="B76">
-        <v>2708</v>
+        <v>2737824</v>
       </c>
       <c r="C76" t="str">
-        <v>2020-01-24 08:46</v>
+        <v>2020-02-15 14:40</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
-        <v>湖北省省长王晓东：关闭离汉通道是以短暂的困难 换取长久平安</v>
+        <v>农民工返程客运总量为3亿人次，目前已返程8000万人次</v>
       </c>
       <c r="B77">
-        <v>221891</v>
+        <v>6257</v>
       </c>
       <c r="C77" t="str">
-        <v>2020-01-24 00:27</v>
+        <v>2020-02-15 14:38</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
-        <v>中国疾控中心主任高福：传染源头就是野生动物 号召大家不要吃野味</v>
+        <v>日本一天内多地确诊新冠肺炎 国内担忧病毒已“隐形暴发”</v>
       </c>
       <c r="B78">
-        <v>1780644</v>
+        <v>53755</v>
       </c>
       <c r="C78" t="str">
-        <v>2020-01-23 23:33</v>
+        <v>2020-02-15 14:30</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
-        <v>疾控中心主任高福：该病毒有特殊的地方，但定会比SARS致死率低</v>
+        <v>美众议长宣扬华为威胁论 傅莹现场反驳：西方民主制度如此脆弱？</v>
       </c>
       <c r="B79">
-        <v>3643468</v>
+        <v>278886</v>
       </c>
       <c r="C79" t="str">
-        <v>2020-01-23 23:28</v>
+        <v>2020-02-15 14:21</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
-        <v>该如何保护自己不被传染？疾控中心主任高福：倡导“口罩文化”</v>
+        <v>泪目！杭州一医院两小时113名医护报名献血：看名单要划屏幕很久</v>
       </c>
       <c r="B80">
-        <v>252700</v>
+        <v>2351</v>
       </c>
       <c r="C80" t="str">
-        <v>2020-01-23 23:18</v>
+        <v>2020-02-15 14:16</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
-        <v>疾控中心主任高福：武汉采取管控措施目的是使病例从武汉输出为零</v>
+        <v>口罩没了怎么办？港大深圳医院教你应急自制：效果达外科口罩九成</v>
       </c>
       <c r="B81">
-        <v>222095</v>
+        <v>66012</v>
       </c>
       <c r="C81" t="str">
-        <v>2020-01-23 23:15</v>
+        <v>2020-02-15 14:08</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
-        <v>网传武汉蔬菜涨价大白菜30元一颗？涉事公司回应 监管部门约谈</v>
+        <v>实拍全球多地蝗灾现场 虫群遮天蔽日已致上千万人受灾</v>
       </c>
       <c r="B82">
-        <v>154233</v>
+        <v>3764797</v>
       </c>
       <c r="C82" t="str">
-        <v>2020-01-23 21:27</v>
+        <v>2020-02-15 11:41</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
-        <v>不计报酬 无论生死！武汉江夏30多名医务人员写请战书上疫情前线</v>
+        <v>王贺胜：疫情防控到了最关键阶段 确保不出现第二个武汉</v>
       </c>
       <c r="B83">
-        <v>88974</v>
+        <v>12717</v>
       </c>
       <c r="C83" t="str">
-        <v>2020-01-23 21:18</v>
+        <v>2020-02-15 11:32</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
-        <v>武汉防疫一线年轻护士：万一的感染话...我的同事会救我的</v>
+        <v>央行：已向武汉紧急调拨40亿新钞 银行现金须消毒后再投放客户</v>
       </c>
       <c r="B84">
-        <v>1749738</v>
+        <v>392536</v>
       </c>
       <c r="C84" t="str">
-        <v>2020-01-23 13:14</v>
+        <v>2020-02-15 11:23</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
-        <v>马克龙动怒大声斥责以色列安保人员：给我出去！</v>
+        <v>中国银保监会：银行业为抗击疫情提供信贷支持超5370亿元</v>
       </c>
       <c r="B85">
-        <v>19080</v>
+        <v>19649</v>
       </c>
       <c r="C85" t="str">
-        <v>2020-01-23 10:53</v>
+        <v>2020-02-15 10:58</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
-        <v>联合国秘书长秀中文拜年：感谢中国人民的支持</v>
+        <v>王贺胜：9个方舱医院收治5606名患者，将确保未收治患者清零</v>
       </c>
       <c r="B86">
-        <v>9767</v>
+        <v>8444</v>
       </c>
       <c r="C86" t="str">
-        <v>2020-01-23 08:15</v>
+        <v>2020-02-15 10:51</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
-        <v>武汉加油！致敬冲在一线的白衣战士：医护病患的同时，请护好自己</v>
+        <v>国家卫健委：湖北防控工作到了最吃紧的时候，呈胶着对垒状态</v>
       </c>
       <c r="B87">
-        <v>11145</v>
+        <v>6215</v>
       </c>
       <c r="C87" t="str">
-        <v>2020-01-23 07:21</v>
+        <v>2020-02-15 10:37</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
-        <v>“我自愿报名，如有需要随叫随到！”此刻，这些医生的话令人泪目</v>
+        <v>重症患者治疗初显成效 武汉市金银潭和肺科医院出院率超30%</v>
       </c>
       <c r="B88">
-        <v>161114</v>
+        <v>174713</v>
       </c>
       <c r="C88" t="str">
-        <v>2020-01-23 06:40</v>
+        <v>2020-02-15 10:31</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
-        <v>杭州一小区近20户人家门口出现神秘符号 民警调查后真相有些暖</v>
+        <v>澳门：不想增加国家负担，采购的口罩主要来自海外</v>
       </c>
       <c r="B89">
-        <v>871881</v>
+        <v>71031</v>
       </c>
       <c r="C89" t="str">
-        <v>2020-01-23 06:30</v>
+        <v>2020-02-15 10:15</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
-        <v>今日起武汉全市公共交通停运！机场、火车站离汉通道暂时关闭</v>
+        <v>湖北：一半以上确诊病例使用中医药治疗 已派出中医医疗队2220人</v>
       </c>
       <c r="B90">
-        <v>1004935</v>
+        <v>38016</v>
       </c>
       <c r="C90" t="str">
-        <v>2020-01-23 06:18</v>
+        <v>2020-02-15 10:02</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
-        <v>新型冠状病毒肺炎已致湖北17人死亡！目前全省累计确诊病例444例</v>
+        <v>王贺胜：各地共派25633名医疗队员 调动医疗救援规模速度超汶川救援</v>
       </c>
       <c r="B91">
-        <v>35384</v>
+        <v>21605</v>
       </c>
       <c r="C91" t="str">
-        <v>2020-01-22 23:21</v>
+        <v>2020-02-15 09:46</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
-        <v>暖心！新型冠状病毒来袭 武汉姐弟开车送老人、警察口罩</v>
+        <v>乘客机场丢下小白箱撒腿就跑 执勤民警当场懵了，打开后深受感动</v>
       </c>
       <c r="B92">
-        <v>232271</v>
+        <v>46925</v>
       </c>
       <c r="C92" t="str">
-        <v>2020-01-22 20:45</v>
+        <v>2020-02-15 09:42</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
-        <v>李兰娟院士谈新型冠状病毒：怕酒精不耐高温 含氯消毒剂可灭活病毒</v>
+        <v>敬礼！浙江453人出征武汉，交警自发列队送“战士”出征</v>
       </c>
       <c r="B93">
-        <v>68513</v>
+        <v>233056</v>
       </c>
       <c r="C93" t="str">
-        <v>2020-01-22 20:17</v>
+        <v>2020-02-15 09:19</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
-        <v>110秒带你认识新型冠状病毒肺炎</v>
+        <v>稀释1000倍仍测出阳性！钟南山指导研发试剂盒：可与核酸检测互补</v>
       </c>
       <c r="B94">
-        <v>146988</v>
+        <v>334063</v>
       </c>
       <c r="C94" t="str">
-        <v>2020-01-22 17:42</v>
+        <v>2020-02-15 08:54</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
-        <v>武大中南医院用ECMO技术成功救治一50岁新型肺炎患者</v>
+        <v>护士哄隔离区新生儿入睡：不怕不怕 我们都在这儿</v>
       </c>
       <c r="B95">
-        <v>72535</v>
+        <v>112661</v>
       </c>
       <c r="C95" t="str">
-        <v>2020-01-22 17:39</v>
+        <v>2020-02-15 08:04</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
-        <v>便衣警察遭暴徒持械围殴 过路市民用身体拼死保护！</v>
+        <v>方舱医院又一患者出院，病友纷纷前来道别：吃完饭再走吧</v>
       </c>
       <c r="B96">
-        <v>7370</v>
+        <v>317552</v>
       </c>
       <c r="C96" t="str">
-        <v>2020-01-22 16:48</v>
+        <v>2020-02-15 07:28</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
-        <v>四川阿坝发生4.5级地震 消防1车3人赴震中 557车330人集结待命</v>
+        <v>河南副省长对话白岩松：确诊第1例时，河南已做好超千例的准备</v>
       </c>
       <c r="B97">
-        <v>11632</v>
+        <v>48210</v>
       </c>
       <c r="C97" t="str">
-        <v>2020-01-22 16:43</v>
+        <v>2020-02-15 07:23</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
-        <v>追踪武汉肺炎疫情发生的24天：确认人传人发生 确诊440余个病例</v>
+        <v>黑龙江首发驰援湖北3000吨大米专列 湖北网友连连道谢：感谢老铁</v>
       </c>
       <c r="B98">
-        <v>17724</v>
+        <v>449204</v>
       </c>
       <c r="C98" t="str">
-        <v>2020-01-22 14:59</v>
+        <v>2020-02-15 07:15</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
-        <v>老外在超市突然用中文高歌 身后买年货的大妈表情亮了</v>
+        <v>湖北一医护妻子回乡支援一线 丈夫托民警送礼物 背后故事让人泪目</v>
       </c>
       <c r="B99">
-        <v>14343</v>
+        <v>66942</v>
       </c>
       <c r="C99" t="str">
-        <v>2020-01-22 13:19</v>
+        <v>2020-02-15 07:08</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
-        <v>早期信息披露不够瞒报疫情？国家卫健委回应</v>
+        <v>面对无人机喊话，婆婆举双手“投降”  喊话员忙解释：我是大好人</v>
       </c>
       <c r="B100">
-        <v>18037</v>
+        <v>1041390</v>
       </c>
       <c r="C100" t="str">
-        <v>2020-01-22 12:26</v>
+        <v>2020-02-15 07:04</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
-        <v>致敬最美逆行者！国家卫健委：疫情发生后医护人员默默坚守在一线</v>
+        <v>“中国必胜，武汉加油！”武昌方舱医院医患集体表白中国武汉</v>
       </c>
       <c r="B101">
-        <v>102592</v>
+        <v>23589</v>
       </c>
       <c r="C101" t="str">
-        <v>2020-01-22 11:54</v>
+        <v>2020-02-14 23:05</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
-        <v>国家卫健委：新型冠状病毒的来源是野生动物，儿童不易感染</v>
+        <v>中医科学院院长：湖北确诊病例中医药参与率超75% 其他地区超90%</v>
       </c>
       <c r="B102">
-        <v>159996</v>
+        <v>15448</v>
       </c>
       <c r="C102" t="str">
-        <v>2020-01-22 11:38</v>
+        <v>2020-02-14 23:02</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
-        <v>中国疾控中心：暂无证据证明已出现“超级传播者”，会密切关注</v>
+        <v>血浆治疗是否存在风险?金银潭医院院长：风险远小于获益</v>
       </c>
       <c r="B103">
-        <v>1515602</v>
+        <v>335754</v>
       </c>
       <c r="C103" t="str">
-        <v>2020-01-22 11:27</v>
+        <v>2020-02-14 22:46</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
-        <v>国家卫健委：新型肺炎病毒有变异的可能，疫情或进一步扩散</v>
+        <v>中医药专家回应方舱医院内打太极拳：增强体质 对患者有益</v>
       </c>
       <c r="B104">
-        <v>165450</v>
+        <v>178110</v>
       </c>
       <c r="C104" t="str">
-        <v>2020-01-22 11:04</v>
+        <v>2020-02-14 22:44</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
-        <v>国家卫健委：新型冠状病毒肺炎确诊440例，死亡9例</v>
+        <v>专家：一旦得新冠肺炎 应该第一时间吃上中药</v>
       </c>
       <c r="B105">
-        <v>15429</v>
+        <v>22961</v>
       </c>
       <c r="C105" t="str">
-        <v>2020-01-22 10:36</v>
+        <v>2020-02-14 22:06</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
-        <v>“不计报酬，无论生死!” 全副武装的白衣战士挡在疫情之前</v>
+        <v>驰援武汉的“抗非”英雄张忠德：中西医协同起效，提高了救治率</v>
       </c>
       <c r="B106">
-        <v>38768</v>
+        <v>12478</v>
       </c>
       <c r="C106" t="str">
-        <v>2020-01-22 10:25</v>
+        <v>2020-02-14 22:04</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
-        <v>男子拄双拐无证醉驾被查：把我关进去吧，心情不好不想回家</v>
+        <v>140秒解密顺丰7199抗疫航班在风雪中，如何提前28分钟到达武汉</v>
       </c>
       <c r="B107">
-        <v>9607</v>
+        <v>76439</v>
       </c>
       <c r="C107" t="str">
-        <v>2020-01-22 09:47</v>
+        <v>2020-02-14 21:52</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
-        <v>美国确诊首例新型肺炎病例，患者曾赴武汉周边地区旅行</v>
+        <v>全国中医药系统向湖北派2220人 多人参与抗击非典</v>
       </c>
       <c r="B108">
-        <v>38856</v>
+        <v>22244</v>
       </c>
       <c r="C108" t="str">
-        <v>2020-01-22 08:06</v>
+        <v>2020-02-14 21:46</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
-        <v>美国国会参议院正式审理总统弹劾案 特朗普远在瑞士不忘发推怼人</v>
+        <v>男子解除隔离后当场跳舞：我要去楼下跑几圈！</v>
       </c>
       <c r="B109">
-        <v>9702</v>
+        <v>24879</v>
       </c>
       <c r="C109" t="str">
-        <v>2020-01-22 07:03</v>
+        <v>2020-02-14 21:06</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
-        <v>不允许发“疫情财”！淘宝发布公告：平台口罩货源充足、绝不涨价</v>
+        <v>甘肃“鸡司令”率千只鸡神走位竟拼出四个大字：中国加油</v>
       </c>
       <c r="B110">
-        <v>33565</v>
+        <v>10109</v>
       </c>
       <c r="C110" t="str">
-        <v>2020-01-22 06:49</v>
+        <v>2020-02-14 19:07</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
-        <v>国士无双！钟南山为防疫工作连轴转5天 84岁老人再赴前线义无反顾</v>
+        <v>没有鲜花只有真心话！武汉病房里八旬夫妻这样驱魔渡劫</v>
       </c>
       <c r="B111">
-        <v>1538618</v>
+        <v>1442289</v>
       </c>
       <c r="C111" t="str">
-        <v>2020-01-22 06:42</v>
+        <v>2020-02-14 18:57</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
-        <v>暖心又霸气！外交部发言人拜年语录：无论走到哪里，祖国在你身后</v>
+        <v>长颈鹿去医院看病？女子穿充气服去医院挂号、拿药：口罩用太久了</v>
       </c>
       <c r="B112">
-        <v>547058</v>
+        <v>4459</v>
       </c>
       <c r="C112" t="str">
-        <v>2020-01-22 06:35</v>
+        <v>2020-02-14 18:20</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
-        <v>欧阳夏丹：面对疫情不可掉以轻心 防控是保护自己，也是对社会负责</v>
+        <v>中国疾控中心专家：外出归来要对手机消毒</v>
       </c>
       <c r="B113">
-        <v>358952</v>
+        <v>16978</v>
       </c>
       <c r="C113" t="str">
-        <v>2020-01-22 02:48</v>
+        <v>2020-02-14 17:44</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
-        <v>疑似病例香港百余人远多广东？港媒挖坑追问，钟南山指偏纠误</v>
+        <v>终于靠岸！海上漂泊12日，“威士特丹”号乘客在柬埔寨获准下船</v>
       </c>
       <c r="B114">
-        <v>1889772</v>
+        <v>4937</v>
       </c>
       <c r="C114" t="str">
-        <v>2020-01-22 01:38</v>
+        <v>2020-02-14 17:23</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
-        <v>快讯！北京今日新增5例新型肺炎病例！患者均于近期前往武汉</v>
+        <v>实拍湖北黄冈街头：景区干道无人如空城 居民间隔一米定点排队购物</v>
       </c>
       <c r="B115">
-        <v>78875</v>
+        <v>491056</v>
       </c>
       <c r="C115" t="str">
-        <v>2020-01-21 23:52</v>
+        <v>2020-02-14 17:18</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
-        <v>转发了解！武汉新型肺炎的潜伏期平均在7天左右</v>
+        <v>财政部：中央财政投入172.9亿元用于疫情防控，主要投向四大方面</v>
       </c>
       <c r="B116">
-        <v>275735</v>
+        <v>2047</v>
       </c>
       <c r="C116" t="str">
-        <v>2020-01-21 22:41</v>
+        <v>2020-02-14 17:04</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
-        <v>湖南破获非法经营野生动物案 查获蛇豹猫鹰等2万多斤</v>
+        <v>国家卫健委：歧视孤立一线医务人员及其家属 情节严重将依法处理</v>
       </c>
       <c r="B117">
-        <v>40423</v>
+        <v>4567</v>
       </c>
       <c r="C117" t="str">
-        <v>2020-01-21 22:09</v>
+        <v>2020-02-14 16:42</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
-        <v>医务人员出现感染情况怎么办？武汉疫情防控指挥部这样解答</v>
+        <v>美军巡逻队射杀叙利亚平民致1死1伤 俄军赶到平息局势</v>
       </c>
       <c r="B118">
-        <v>96591</v>
+        <v>24777</v>
       </c>
       <c r="C118" t="str">
-        <v>2020-01-21 20:26</v>
+        <v>2020-02-14 16:24</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
-        <v>广东确诊14例新型冠状病毒感染肺炎病例，公布30家定点收治医院</v>
+        <v>湖北女警为防疫工作通宵执勤昏倒路中央 离家只剩不到500米</v>
       </c>
       <c r="B119">
-        <v>9992</v>
+        <v>212249</v>
       </c>
       <c r="C119" t="str">
-        <v>2020-01-21 20:24</v>
+        <v>2020-02-14 16:18</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
-        <v>武汉市长呼吁：外面的人不要到武汉，市民没特殊情况也别出武汉</v>
+        <v>为保障医务人员权益 这些政策将向防疫一线倾斜</v>
       </c>
       <c r="B120">
-        <v>41558</v>
+        <v>4724</v>
       </c>
       <c r="C120" t="str">
-        <v>2020-01-21 20:19</v>
+        <v>2020-02-14 16:12</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
-        <v>我酸了！海军兵哥哥战舰上求婚 表白、求婚等“科目”陆续展开……</v>
+        <v>医护过劳晕倒有无改善？国家卫健委回应</v>
       </c>
       <c r="B121">
-        <v>9101</v>
+        <v>2299</v>
       </c>
       <c r="C121" t="str">
-        <v>2020-01-21 20:15</v>
+        <v>2020-02-14 15:48</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
-        <v>马英九化身"外卖小哥"送祝福 订餐民众惊喜直呼：什么情况？！</v>
+        <v>前线医务人员心理压力如何疏导？卫健委称已采取一系列这样的措施</v>
       </c>
       <c r="B122">
-        <v>5878</v>
+        <v>1977</v>
       </c>
       <c r="C122" t="str">
-        <v>2020-01-21 20:12</v>
+        <v>2020-02-14 15:37</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
-        <v>新型冠状病毒防控：正确佩戴口罩可降低感染风险</v>
+        <v>寒潮来袭！防疫民警执勤花式御寒：跺脚、跳舞、打军体拳……</v>
       </c>
       <c r="B123">
-        <v>160033</v>
+        <v>23087</v>
       </c>
       <c r="C123" t="str">
-        <v>2020-01-21 20:02</v>
+        <v>2020-02-14 15:29</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
-        <v>武汉：除3家定点医院800个床位外 再腾出1200个收治肺炎病人</v>
+        <v>财政部：确保人民群众不因担心费用问题而不敢就诊</v>
       </c>
       <c r="B124">
-        <v>13491</v>
+        <v>95496</v>
       </c>
       <c r="C124" t="str">
-        <v>2020-01-21 19:53</v>
+        <v>2020-02-14 15:19</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
-        <v>武汉：确保肺炎病人得到收诊治疗 住院病人和门诊病人基本零负担</v>
+        <v>无湖北接触史是如何感染的 ？来自天津的警报：危险传播链超乎想象！</v>
       </c>
       <c r="B125">
-        <v>50207</v>
+        <v>5775981</v>
       </c>
       <c r="C125" t="str">
-        <v>2020-01-21 19:47</v>
+        <v>2020-02-14 15:12</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
-        <v>钟南山：要关注非传染病科的医护人员 不要让他们变成传染源</v>
+        <v>国家卫健委：全国已报告医务人员确诊病例1716例，死亡6例</v>
       </c>
       <c r="B126">
-        <v>463309</v>
+        <v>18189</v>
       </c>
       <c r="C126" t="str">
-        <v>2020-01-21 18:57</v>
+        <v>2020-02-14 15:05</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
-        <v>钟南山：赞成发烧人员禁止离开武汉的措施，遏制疫情扩散！</v>
+        <v>民警防疫巡查发现人员聚集欲劝诫 进入屋内后意外查到两名逃犯</v>
       </c>
       <c r="B127">
-        <v>64087</v>
+        <v>49305</v>
       </c>
       <c r="C127" t="str">
-        <v>2020-01-21 18:37</v>
+        <v>2020-02-14 14:28</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
-        <v>钟南山：新型冠状病毒肺炎暂无特效药，最担心出现超级传播者</v>
+        <v>印度大批男子翻入女校内猥亵学生 目击者：男子满校园围追女生</v>
       </c>
       <c r="B128">
-        <v>169071</v>
+        <v>2043343</v>
       </c>
       <c r="C128" t="str">
-        <v>2020-01-21 18:20</v>
+        <v>2020-02-14 14:18</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
-        <v>世卫组织将召开会议评估疫情 外交部：中方愿与国际社会携手应对</v>
+        <v>连线看守所，疫情期间法院通过微信群视频“隔空”审刑犯</v>
       </c>
       <c r="B129">
-        <v>92939</v>
+        <v>5128</v>
       </c>
       <c r="C129" t="str">
-        <v>2020-01-21 17:19</v>
+        <v>2020-02-14 14:12</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
-        <v>港警“一哥”听了都说好！市民组织撑警音乐会 支持警察止暴制乱</v>
+        <v>嚣张！男子遛狗不戴口罩 自称“特种部队”并推搡执法人员</v>
       </c>
       <c r="B130">
-        <v>12829</v>
+        <v>259970</v>
       </c>
       <c r="C130" t="str">
-        <v>2020-01-21 16:21</v>
+        <v>2020-02-14 14:11</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
-        <v>战胜呼吸道疾病，预防性消毒很管用</v>
+        <v>出狱当天跟朋友聚餐喝酒，出小区时偷翻大门被拘了</v>
       </c>
       <c r="B131">
-        <v>8357</v>
+        <v>190306</v>
       </c>
       <c r="C131" t="str">
-        <v>2020-01-21 15:21</v>
+        <v>2020-02-14 13:48</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
-        <v>蔡英文自曝：爸爸若在世或不让我“大选” 网友神补刀：现在该听话了</v>
+        <v>乌克兰4名醉酒男子开车迷路 争执方向时一人引爆手榴弹，现场惨烈</v>
       </c>
       <c r="B132">
-        <v>65943</v>
+        <v>604223</v>
       </c>
       <c r="C132" t="str">
-        <v>2020-01-21 12:51</v>
+        <v>2020-02-14 13:44</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
-        <v>蔡英文连任后嚣张至极 外交部长王毅强硬回应统一决心绝不动摇</v>
+        <v>用虚假口罩信息诈骗钱财网络赌博！男子被判刑2年8个月</v>
       </c>
       <c r="B133">
-        <v>399350</v>
+        <v>76389</v>
       </c>
       <c r="C133" t="str">
-        <v>2020-01-21 12:07</v>
+        <v>2020-02-14 13:32</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
-        <v>现场！男子高速路上疲劳驾驶 一个急刹车刮地起白烟漂了几十米</v>
+        <v>及时雨！澳大利亚林火危机终结 重灾区新南威尔士州火势得到控制</v>
       </c>
       <c r="B134">
-        <v>15582</v>
+        <v>68792</v>
       </c>
       <c r="C134" t="str">
-        <v>2020-01-21 11:27</v>
+        <v>2020-02-14 12:36</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
-        <v>王毅：中美关系牵动世界走向，两国合则两利斗则俱伤</v>
+        <v>掐断病毒源！天津通过禁食野生动物决定：食用者最高处10倍罚款</v>
       </c>
       <c r="B135">
-        <v>12782</v>
+        <v>67134</v>
       </c>
       <c r="C135" t="str">
-        <v>2020-01-21 11:27</v>
+        <v>2020-02-14 12:31</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
-        <v>引渡案在温哥华开庭：有围观者现场拜年送祝福，孟晚舟微笑致谢</v>
+        <v>叙利亚政府军直升机被击落：空中分解成碎片，致2人死亡</v>
       </c>
       <c r="B136">
-        <v>85019</v>
+        <v>112662</v>
       </c>
       <c r="C136" t="str">
-        <v>2020-01-21 10:07</v>
+        <v>2020-02-14 12:29</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
-        <v>引渡案听证会再开庭：孟晚舟脚戴电子镣铐，面带自信微笑出庭</v>
+        <v>疫线医生夫妻科室相距不足百米却十多天没见 隔墙问候纸笔传情</v>
       </c>
       <c r="B137">
-        <v>94352</v>
+        <v>41053</v>
       </c>
       <c r="C137" t="str">
-        <v>2020-01-21 09:10</v>
+        <v>2020-02-14 11:33</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
-        <v>高速秀恩爱！司机边开车边吃老婆喂的橘子 结果车翻了</v>
+        <v>80后夫妻相识“非典”战场，如今携手再战疫情：目的一致，战必胜</v>
       </c>
       <c r="B138">
-        <v>356362</v>
+        <v>7095</v>
       </c>
       <c r="C138" t="str">
-        <v>2020-01-21 09:03</v>
+        <v>2020-02-14 11:31</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
-        <v>这就是传承！看着爸爸越走越远 年幼的女儿向背影敬了一个军礼</v>
+        <v>画面曝光！南美杀手扮成警察由真警察带路进入病房暗杀送医囚犯</v>
       </c>
       <c r="B139">
-        <v>32198</v>
+        <v>19980</v>
       </c>
       <c r="C139" t="str">
-        <v>2020-01-21 07:44</v>
+        <v>2020-02-14 11:31</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
-        <v>人才！男子偷外卖被抓后上演实力“报菜名” 民警：越说越饿！</v>
+        <v>男子不配合防疫工作获刑七个月 身穿防护服出庭受审</v>
       </c>
       <c r="B140">
-        <v>107664</v>
+        <v>22332</v>
       </c>
       <c r="C140" t="str">
-        <v>2020-01-21 07:35</v>
+        <v>2020-02-14 11:30</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
-        <v>萌化了！威风凛凛的缉毒犬见到兽医拿着针管 一秒埋进主人怀里</v>
+        <v>泪目！抗疫护士与男友隔着玻璃亲吻，深情对话感动网友</v>
       </c>
       <c r="B141">
-        <v>56545</v>
+        <v>861668</v>
       </c>
       <c r="C141" t="str">
-        <v>2020-01-21 07:05</v>
+        <v>2020-02-14 11:30</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
-        <v>突发！伊拉克首都美国使馆区附近遭3枚火箭弹袭击 防空警报长鸣</v>
+        <v>“日本最美女孩”到中国驻日使馆转交善款 大使题字：万里尚为邻</v>
       </c>
       <c r="B142">
-        <v>25202</v>
+        <v>16369</v>
       </c>
       <c r="C142" t="str">
-        <v>2020-01-21 06:53</v>
+        <v>2020-02-14 11:23</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
-        <v>阻碍执法、恐吓警员、辱骂一哥……起底香港纵暴议员的无耻行径！</v>
+        <v>逾80岁女性，未有出国经历！日本境内首例新冠肺炎死亡病例</v>
       </c>
       <c r="B143">
-        <v>47931</v>
+        <v>9183</v>
       </c>
       <c r="C143" t="str">
-        <v>2020-01-21 06:42</v>
+        <v>2020-02-14 11:19</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
-        <v>钟南山：新型冠状病毒呈现人传人特点 14名医护人员感染</v>
+        <v>逃亡5年窃贼因疫情乖乖投案：藏匿地点常有人检查，绝望了</v>
       </c>
       <c r="B144">
-        <v>377902</v>
+        <v>10610</v>
       </c>
       <c r="C144" t="str">
-        <v>2020-01-20 23:39</v>
+        <v>2020-02-14 11:07</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
-        <v>如何预防新型冠状病毒？钟南山表示不一定非戴N95口罩</v>
+        <v>事发下班高峰！美国华盛顿发生枪击案 致1死1伤，嫌犯被捕</v>
       </c>
       <c r="B145">
-        <v>752673</v>
+        <v>14661</v>
       </c>
       <c r="C145" t="str">
-        <v>2020-01-20 23:34</v>
+        <v>2020-02-14 10:58</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
-        <v>钟南山：新型冠状病毒肺炎很可能来自野味</v>
+        <v>鱼水一家人！得知“老陕爱吃面”他们就给陕西援鄂医生做油泼辣子面</v>
       </c>
       <c r="B146">
-        <v>873074</v>
+        <v>20325</v>
       </c>
       <c r="C146" t="str">
-        <v>2020-01-20 22:58</v>
+        <v>2020-02-14 10:49</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
-        <v>我来给你们看病！朝阳医院医生被砍后，同事上前接力诊治患者</v>
+        <v>38亿美元！美国防部调整武器预算 用于美墨边境墙建设</v>
       </c>
       <c r="B147">
-        <v>430403</v>
+        <v>18953</v>
       </c>
       <c r="C147" t="str">
-        <v>2020-01-20 22:47</v>
+        <v>2020-02-14 10:07</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
-        <v>钟南山：新型冠状病毒传染性比SARS弱</v>
+        <v>感觉好就画彩虹！无人机温柔询问老人身体状况 隔空对跳野狼disco</v>
       </c>
       <c r="B148">
-        <v>279838</v>
+        <v>599538</v>
       </c>
       <c r="C148" t="str">
-        <v>2020-01-20 22:42</v>
+        <v>2020-02-14 10:04</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
-        <v>山火、暴雨、冰雹、雷暴后 澳大利亚再遭20米高红色沙尘暴</v>
+        <v>援鄂护士防控一线过生日 同事手绘蛋糕 隔窗合唱生日歌</v>
       </c>
       <c r="B149">
-        <v>2399</v>
+        <v>77030</v>
       </c>
       <c r="C149" t="str">
-        <v>2020-01-20 22:41</v>
+        <v>2020-02-14 09:53</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
-        <v>钟南山：新型冠状病毒肺炎肯定存在人传人现象</v>
+        <v>女子不戴口罩又串门被劝阻，叫嚣：拘留我吧，正好没地方吃饭</v>
       </c>
       <c r="B150">
-        <v>76595</v>
+        <v>603303</v>
       </c>
       <c r="C150" t="str">
-        <v>2020-01-20 22:38</v>
+        <v>2020-02-14 09:42</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
-        <v>暴徒非法集会高呼“黑警”口号 正义男子反驳：求你们动动脑子</v>
+        <v>“白色情人节”北京降下鹅毛大雪 多区已被积雪覆盖</v>
       </c>
       <c r="B151">
-        <v>297390</v>
+        <v>1029232</v>
       </c>
       <c r="C151" t="str">
-        <v>2020-01-20 22:29</v>
+        <v>2020-02-14 09:18</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
-        <v>泪目！穿越一万多公里 72岁老人与援助苏丹儿子隔空分享年味</v>
+        <v>新冠肺炎痊愈患者发声：我愿意捐献血浆为疫情做点事</v>
       </c>
       <c r="B152">
-        <v>38978</v>
+        <v>65495</v>
       </c>
       <c r="C152" t="str">
-        <v>2020-01-20 17:52</v>
+        <v>2020-02-14 08:53</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
-        <v>美国夏威夷枪击案：凶手刀刺房东，枪杀2名警察后纵火</v>
+        <v>愿归来平安！100秒情人节祝福献给抗疫夫妻档</v>
       </c>
       <c r="B153">
-        <v>3969</v>
+        <v>267320</v>
       </c>
       <c r="C153" t="str">
-        <v>2020-01-20 17:38</v>
+        <v>2020-02-14 06:47</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
-        <v>耿爽：将同各方携手应对武汉肺炎疫情 共同维护地区和全球卫生安全</v>
+        <v>糊涂男子为“蹭吃蹭住”谎称从武汉返回，隔离14天后被拘</v>
       </c>
       <c r="B154">
-        <v>135139</v>
+        <v>220304</v>
       </c>
       <c r="C154" t="str">
-        <v>2020-01-20 16:46</v>
+        <v>2020-02-14 04:00</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
-        <v>尴尬！约翰逊下车时车门怎么也打不开 默克尔站在门外看着这一切</v>
+        <v>医护人员在方舱医院带患者打太极拳 还有患者自己做起俯卧撑</v>
       </c>
       <c r="B155">
-        <v>69527</v>
+        <v>21410</v>
       </c>
       <c r="C155" t="str">
-        <v>2020-01-20 15:15</v>
+        <v>2020-02-14 03:13</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
-        <v>男子因家庭矛盾劫持8人欲逐一杀害 被武警破门而入空手夺刀制服</v>
+        <v>无证棋牌室聚集16人 女民警现场怼哭打牌人员</v>
       </c>
       <c r="B156">
-        <v>148416</v>
+        <v>214395</v>
       </c>
       <c r="C156" t="str">
-        <v>2020-01-20 15:11</v>
+        <v>2020-02-14 01:30</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
-        <v>温馨！云南瑞丽出入境边防检查站装点中国红欢迎游子回家过年</v>
+        <v>重症患者血液粪便中找到病毒 专家：可能出现其他病毒传播途径</v>
       </c>
       <c r="B157">
-        <v>2324</v>
+        <v>4931</v>
       </c>
       <c r="C157" t="str">
-        <v>2020-01-20 15:02</v>
+        <v>2020-02-13 22:54</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
-        <v>武汉疾控专家手把手教您如何正确的佩戴口罩和洗手</v>
+        <v>华中科技大学同济医院院长王伟：临床诊断病例纳入确诊是好消息</v>
       </c>
       <c r="B158">
-        <v>103820</v>
+        <v>985404</v>
       </c>
       <c r="C158" t="str">
-        <v>2020-01-20 14:01</v>
+        <v>2020-02-13 22:48</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
-        <v>董浩送别赵忠祥：死在舞台上是主持人最高境界，他做到了，是个爷们儿</v>
+        <v>轻症患者符合什么标准要转诊到重症定点医院？专家回应了这几点</v>
       </c>
       <c r="B159">
-        <v>348471</v>
+        <v>103569</v>
       </c>
       <c r="C159" t="str">
-        <v>2020-01-20 11:44</v>
+        <v>2020-02-13 22:42</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
-        <v>马斯克创造航天新壮举！自爆升空火箭后成功实现载人舱逃逸</v>
+        <v>专家：与SARS相比，新冠肺炎患者病情进展更快、心脏受攻击更厉害</v>
       </c>
       <c r="B160">
-        <v>7338</v>
+        <v>408591</v>
       </c>
       <c r="C160" t="str">
-        <v>2020-01-20 09:26</v>
+        <v>2020-02-13 22:41</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
-        <v>德国外长批特朗普对伊朗“极限施压”：我们不会跟随美国</v>
+        <v>金银潭医院院长：患者康复后体内有抗体，恳请他们伸出胳膊捐献血浆</v>
       </c>
       <c r="B161">
-        <v>5050</v>
+        <v>100399</v>
       </c>
       <c r="C161" t="str">
-        <v>2020-01-20 07:17</v>
+        <v>2020-02-13 22:12</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
-        <v>港警：主办方挑衅致乱港集会升级为暴动，至少2名警员被围殴</v>
+        <v>诊断标准中为何增加临床诊断病例？中央指导组医疗救治组专家回应</v>
       </c>
       <c r="B162">
-        <v>12621</v>
+        <v>5608</v>
       </c>
       <c r="C162" t="str">
-        <v>2020-01-20 07:13</v>
+        <v>2020-02-13 22:09</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
-        <v>消防员车内挂点滴，有警拔针即出发！网友看完：超心疼</v>
+        <v>“我不想你走”！医务人员出发驰援武汉前一刻 儿子拉住母亲的手…</v>
       </c>
       <c r="B163">
-        <v>126631</v>
+        <v>1146426</v>
       </c>
       <c r="C163" t="str">
-        <v>2020-01-20 07:00</v>
+        <v>2020-02-13 20:52</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
-        <v>时隔11年，“限塑令”迎来升级版! 郭志坚：新规落地必须要刚起来！</v>
+        <v>泪目！妈妈赴汉抗疫，儿子哽咽叮嘱：你一定要照顾好自己，不然怎么照顾他们</v>
       </c>
       <c r="B164">
-        <v>2337</v>
+        <v>3865</v>
       </c>
       <c r="C164" t="str">
-        <v>2020-01-20 06:46</v>
+        <v>2020-02-13 20:44</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="str">
+        <v>按下暂停键的20天，留在武汉的普通人怎样生活？看哭了……</v>
+      </c>
+      <c r="B165">
+        <v>470334</v>
+      </c>
+      <c r="C165" t="str">
+        <v>2020-02-13 19:04</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="str">
+        <v>棉签当蜡烛、鲜花饼当蛋糕…方舱医院内医务人员的别样生日会</v>
+      </c>
+      <c r="B166">
+        <v>12895</v>
+      </c>
+      <c r="C166" t="str">
+        <v>2020-02-13 19:03</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="str">
+        <v>粪便中检出新冠病毒，国家卫健委：不意味着主要传播途径变化</v>
+      </c>
+      <c r="B167">
+        <v>2240</v>
+      </c>
+      <c r="C167" t="str">
+        <v>2020-02-13 18:47</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="str">
+        <v>80岁北大荒奶奶 交5万元特殊党费助力“抗疫”</v>
+      </c>
+      <c r="B168">
+        <v>3380</v>
+      </c>
+      <c r="C168" t="str">
+        <v>2020-02-13 18:40</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="str">
+        <v>国家卫健委：重症和危重症也可治愈 治愈患者中重症危重症占10%</v>
+      </c>
+      <c r="B169">
+        <v>109994</v>
+      </c>
+      <c r="C169" t="str">
+        <v>2020-02-13 18:03</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="str">
+        <v>荒唐！明知聚餐亲戚得了新冠肺炎还不在意，一家7口全部“中招”</v>
+      </c>
+      <c r="B170">
+        <v>627879</v>
+      </c>
+      <c r="C170" t="str">
+        <v>2020-02-13 18:01</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="str">
+        <v>韩国首尔市政府向中国提供的援助物资已启运：该是报恩的时候了</v>
+      </c>
+      <c r="B171">
+        <v>7899</v>
+      </c>
+      <c r="C171" t="str">
+        <v>2020-02-13 17:19</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="str">
+        <v>国家发改委：湖北口罩日产15.8万只 全国口罩产能利用率已达到94%</v>
+      </c>
+      <c r="B172">
+        <v>6631</v>
+      </c>
+      <c r="C172" t="str">
+        <v>2020-02-13 17:02</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="str">
+        <v>台当局推行“口罩实名制限购” 网友：每人每七天买两个，真脑残</v>
+      </c>
+      <c r="B173">
+        <v>51132</v>
+      </c>
+      <c r="C173" t="str">
+        <v>2020-02-13 16:39</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="str">
+        <v>钟南山团队实验室在患者粪便中检出新冠活病毒</v>
+      </c>
+      <c r="B174">
+        <v>65083</v>
+      </c>
+      <c r="C174" t="str">
+        <v>2020-02-13 16:38</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="str">
+        <v>国家卫健委：12日全国新增确诊病例15152例，累计59804例</v>
+      </c>
+      <c r="B175">
+        <v>8486</v>
+      </c>
+      <c r="C175" t="str">
+        <v>2020-02-13 16:34</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="str">
+        <v>山西1省援3市  6批医疗队600余名“逆行者”支援湖北</v>
+      </c>
+      <c r="B176">
+        <v>7142</v>
+      </c>
+      <c r="C176" t="str">
+        <v>2020-02-13 14:55</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="str">
+        <v>兴凯湖地震致冰块上岸？官方辟谣：气温升高造成的一种自然现象</v>
+      </c>
+      <c r="B177">
+        <v>5789</v>
+      </c>
+      <c r="C177" t="str">
+        <v>2020-02-13 14:37</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="str">
+        <v>男子假借卖口罩诈骗爱心人士16万 被捕后这句话让民警怒了</v>
+      </c>
+      <c r="B178">
+        <v>79459</v>
+      </c>
+      <c r="C178" t="str">
+        <v>2020-02-13 14:37</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="str">
+        <v>向社会道歉！汉口银行回应员工穿防护服摆拍：自购非医用防护服</v>
+      </c>
+      <c r="B179">
+        <v>5185</v>
+      </c>
+      <c r="C179" t="str">
+        <v>2020-02-13 13:59</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="str">
+        <v>感动！空军机组录音公开：凯旋时接你们回家</v>
+      </c>
+      <c r="B180">
+        <v>26951</v>
+      </c>
+      <c r="C180" t="str">
+        <v>2020-02-13 12:40</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="str">
+        <v>冷血卑鄙！无视世卫组织命名 台当局借新冠肺炎疫情搞“台独”</v>
+      </c>
+      <c r="B181">
+        <v>141124</v>
+      </c>
+      <c r="C181" t="str">
+        <v>2020-02-13 12:12</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="str">
+        <v>运-20来了！ “胖妞” 首次执行大型非战争军事任务抵达武汉</v>
+      </c>
+      <c r="B182">
+        <v>12063</v>
+      </c>
+      <c r="C182" t="str">
+        <v>2020-02-13 12:07</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="str">
+        <v>现场直击！运-20等多型运输机抵达武汉天河机场</v>
+      </c>
+      <c r="B183">
+        <v>29104</v>
+      </c>
+      <c r="C183" t="str">
+        <v>2020-02-13 10:46</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="str">
+        <v>现场直击！运-20等多型运输机抵达武汉天河机场</v>
+      </c>
+      <c r="B184">
+        <v>1360684</v>
+      </c>
+      <c r="C184" t="str">
+        <v>2020-02-13 10:32</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="str">
+        <v>18.3℃！南极洲气温创近60年来新高</v>
+      </c>
+      <c r="B185">
+        <v>2932</v>
+      </c>
+      <c r="C185" t="str">
+        <v>2020-02-13 10:03</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="str">
+        <v>躲过一劫又飘了？被问从弹劾事件学到什么 特朗普：我支持率很高</v>
+      </c>
+      <c r="B186">
+        <v>40758</v>
+      </c>
+      <c r="C186" t="str">
+        <v>2020-02-13 09:40</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="str">
+        <v>嘉兴首例！棋牌室老板娘拒不配合疫情管控还袭警，被判拘役一个月</v>
+      </c>
+      <c r="B187">
+        <v>27025</v>
+      </c>
+      <c r="C187" t="str">
+        <v>2020-02-13 09:08</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="str">
+        <v>“俄罗斯与中国同在”：俄外交部发言人用中文为中国加油</v>
+      </c>
+      <c r="B188">
+        <v>113633</v>
+      </c>
+      <c r="C188" t="str">
+        <v>2020-02-13 07:47</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="str">
+        <v>最甜的笑脸！火神山医院执勤武警下哨后 摘下口罩瞬间笑容暖哭众人</v>
+      </c>
+      <c r="B189">
+        <v>255794</v>
+      </c>
+      <c r="C189" t="str">
+        <v>2020-02-13 07:46</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="str">
+        <v>新加坡男子录超市试喝饮料扬言散播病毒视频 回传网络惹众怒</v>
+      </c>
+      <c r="B190">
+        <v>108866</v>
+      </c>
+      <c r="C190" t="str">
+        <v>2020-02-13 07:44</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="str">
+        <v>湖北将再建一所应急医院！黄冈疫情最重县计划7天建成“小汤山”</v>
+      </c>
+      <c r="B191">
+        <v>8271991</v>
+      </c>
+      <c r="C191" t="str">
+        <v>2020-02-13 07:05</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="str">
+        <v>已传唤！莆田男子开奔驰被拦村口 下车辱骂、抡锄头殴打防疫人员</v>
+      </c>
+      <c r="B192">
+        <v>7342</v>
+      </c>
+      <c r="C192" t="str">
+        <v>2020-02-13 06:48</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="str">
+        <v>致敬！华西援鄂医护人员查房时 新冠肺炎患者连说5次“非常感谢”</v>
+      </c>
+      <c r="B193">
+        <v>1450458</v>
+      </c>
+      <c r="C193" t="str">
+        <v>2020-02-13 00:41</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="str">
+        <v>抗疫一线医护人员工作状态：穿防护服全身湿透 备的纸尿裤用不到</v>
+      </c>
+      <c r="B194">
+        <v>24672</v>
+      </c>
+      <c r="C194" t="str">
+        <v>2020-02-12 23:01</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="str">
+        <v>中国疾控中心专家：所有消毒剂对新冠病毒都有效</v>
+      </c>
+      <c r="B195">
+        <v>102022</v>
+      </c>
+      <c r="C195" t="str">
+        <v>2020-02-12 22:57</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="str">
+        <v>59岁患者出院对住院病友隔空鼓励：赶紧出院赶紧好！</v>
+      </c>
+      <c r="B196">
+        <v>6111</v>
+      </c>
+      <c r="C196" t="str">
+        <v>2020-02-12 22:47</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="str">
+        <v>工作人员穿防护服摆拍后丢弃 调查：汉口银行志愿者，纪委已介入</v>
+      </c>
+      <c r="B197">
+        <v>2360827</v>
+      </c>
+      <c r="C197" t="str">
+        <v>2020-02-12 21:15</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="str">
+        <v>空姐泪洒贵州援鄂航班 哽咽播报：愿你们平安回家</v>
+      </c>
+      <c r="B198">
+        <v>18440</v>
+      </c>
+      <c r="C198" t="str">
+        <v>2020-02-12 20:42</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="str">
+        <v>男子穿充气宇航服乘坐飞机走红 网友调侃：好厉害的样子</v>
+      </c>
+      <c r="B199">
+        <v>47907</v>
+      </c>
+      <c r="C199" t="str">
+        <v>2020-02-12 20:37</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="str">
+        <v>万众一心！大批港星录视频为武汉加油，向前线战士致敬！</v>
+      </c>
+      <c r="B200">
+        <v>1550876</v>
+      </c>
+      <c r="C200" t="str">
+        <v>2020-02-12 20:23</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="str">
+        <v>葫芦岛一企业爆炸致5死10伤 涉事公司已停产整顿，负责人已被控制</v>
+      </c>
+      <c r="B201">
+        <v>3173</v>
+      </c>
+      <c r="C201" t="str">
+        <v>2020-02-12 20:23</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="str">
+        <v>教育部：湖北学生解除限制后才能去外地返校</v>
+      </c>
+      <c r="B202">
+        <v>15484</v>
+      </c>
+      <c r="C202" t="str">
+        <v>2020-02-12 18:33</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="str">
+        <v>最新数据！教育部：123所高校7924名医护人员支援武汉，向你们致敬！</v>
+      </c>
+      <c r="B203">
+        <v>6985</v>
+      </c>
+      <c r="C203" t="str">
+        <v>2020-02-12 18:27</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="str">
+        <v>ICU护士劳累过度摔倒致鼻梁骨折 仍放弃休息忍痛奋战一线</v>
+      </c>
+      <c r="B204">
+        <v>37972</v>
+      </c>
+      <c r="C204" t="str">
+        <v>2020-02-12 17:10</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="str">
+        <v>各地空管和医疗队专机的对话：期待你们平安凯旋</v>
+      </c>
+      <c r="B205">
+        <v>101149</v>
+      </c>
+      <c r="C205" t="str">
+        <v>2020-02-12 16:49</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="str">
+        <v>硕士研究生复试是否延期？教育部回应</v>
+      </c>
+      <c r="B206">
+        <v>3270</v>
+      </c>
+      <c r="C206" t="str">
+        <v>2020-02-12 16:41</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="str">
+        <v>国家卫健委：新冠肺炎患者治愈比例上升至10.6%</v>
+      </c>
+      <c r="B207">
+        <v>2358</v>
+      </c>
+      <c r="C207" t="str">
+        <v>2020-02-12 16:38</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="str">
+        <v>教育部：特别不提倡、不建议每位高校老师都开网课</v>
+      </c>
+      <c r="B208">
+        <v>5232</v>
+      </c>
+      <c r="C208" t="str">
+        <v>2020-02-12 16:31</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="str">
+        <v>距离高考还有4个月，今年高考会推迟吗？教育部作出回应</v>
+      </c>
+      <c r="B209">
+        <v>23073</v>
+      </c>
+      <c r="C209" t="str">
+        <v>2020-02-12 16:18</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="str">
+        <v>蝙蝠餐在印尼仍热卖 摊贩：经常卖光 甚至库存不足</v>
+      </c>
+      <c r="B210">
+        <v>9630096</v>
+      </c>
+      <c r="C210" t="str">
+        <v>2020-02-12 16:09</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="str">
+        <v>好消息！西藏唯一确诊病例治愈出院 自治区内确诊和疑似病例清零</v>
+      </c>
+      <c r="B211">
+        <v>3592</v>
+      </c>
+      <c r="C211" t="str">
+        <v>2020-02-12 16:09</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="str">
+        <v>大学生返校后是否先隔离14天？教育部回应</v>
+      </c>
+      <c r="B212">
+        <v>13170</v>
+      </c>
+      <c r="C212" t="str">
+        <v>2020-02-12 15:53</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="str">
+        <v>声援新冠肺炎患者，以色列特拉维夫市政厅“点亮”中国国旗！</v>
+      </c>
+      <c r="B213">
+        <v>29512</v>
+      </c>
+      <c r="C213" t="str">
+        <v>2020-02-12 15:17</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="str">
+        <v>现场直击：海南援鄂护理团队带武汉方舱医院患者练八段锦</v>
+      </c>
+      <c r="B214">
+        <v>288046</v>
+      </c>
+      <c r="C214" t="str">
+        <v>2020-02-12 14:58</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="str">
+        <v>疾控专家：若局部病毒很高接触2秒也会传染</v>
+      </c>
+      <c r="B215">
+        <v>87266</v>
+      </c>
+      <c r="C215" t="str">
+        <v>2020-02-12 14:51</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="str">
+        <v>泪崩！火神山医院一护士听闻母亲去世 向家的方向三鞠躬后继续工作</v>
+      </c>
+      <c r="B216">
+        <v>3609686</v>
+      </c>
+      <c r="C216" t="str">
+        <v>2020-02-12 14:51</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="str">
+        <v>尴尬！小区封闭，武汉蔡甸一传销团伙“弹尽粮绝”主动自首</v>
+      </c>
+      <c r="B217">
+        <v>64962</v>
+      </c>
+      <c r="C217" t="str">
+        <v>2020-02-12 14:49</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="str">
+        <v>民航局：飞机已全部配备高效过滤器 可过滤99.9%污染颗粒物</v>
+      </c>
+      <c r="B218">
+        <v>163551</v>
+      </c>
+      <c r="C218" t="str">
+        <v>2020-02-12 14:11</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="str">
+        <v>法国前总理用中文为武汉加油 其曾在“非典”期间坚持访华</v>
+      </c>
+      <c r="B219">
+        <v>2489</v>
+      </c>
+      <c r="C219" t="str">
+        <v>2020-02-12 14:07</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="str">
+        <v>火神山医院患者变身志愿者：推轮椅调电视，只为减轻医护人员压力</v>
+      </c>
+      <c r="B220">
+        <v>270234</v>
+      </c>
+      <c r="C220" t="str">
+        <v>2020-02-12 11:44</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="str">
+        <v>80后夫妻相识“非典”战场，如今携手再战疫情：目的一致，战必胜</v>
+      </c>
+      <c r="B221">
+        <v>713860</v>
+      </c>
+      <c r="C221" t="str">
+        <v>2020-02-12 11:30</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="str">
+        <v>北京首例！小区搭设3.6米“消毒通道”防控疫情</v>
+      </c>
+      <c r="B222">
+        <v>37332</v>
+      </c>
+      <c r="C222" t="str">
+        <v>2020-02-12 10:07</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="str">
+        <v>“钻石公主”号确诊病例增39感染者升至174人  含1名检疫官</v>
+      </c>
+      <c r="B223">
+        <v>15643</v>
+      </c>
+      <c r="C223" t="str">
+        <v>2020-02-12 09:53</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="str">
+        <v>“湖北人民我们非常感谢你们” 仍在病床，他向医护讲了报恩计划</v>
+      </c>
+      <c r="B224">
+        <v>114620</v>
+      </c>
+      <c r="C224" t="str">
+        <v>2020-02-12 09:45</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="str">
+        <v>中央指导组约谈武汉副市长等3人 媒体实拍集中收治当晚混乱一幕</v>
+      </c>
+      <c r="B225">
+        <v>171465</v>
+      </c>
+      <c r="C225" t="str">
+        <v>2020-02-12 09:10</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="str">
+        <v>双双感染新冠肺炎，87岁爷爷举着吊瓶走进隔离病房哄83岁奶奶吃饭</v>
+      </c>
+      <c r="B226">
+        <v>7007882</v>
+      </c>
+      <c r="C226" t="str">
+        <v>2020-02-12 09:01</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="str">
+        <v>90家医疗机构250人！披星戴月，广东第二批医疗队带着物资援荆</v>
+      </c>
+      <c r="B227">
+        <v>15805</v>
+      </c>
+      <c r="C227" t="str">
+        <v>2020-02-12 08:18</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="str">
+        <v>返岗复工后如何做好自我防护？这份防疫宝典请收好！</v>
+      </c>
+      <c r="B228">
+        <v>6777</v>
+      </c>
+      <c r="C228" t="str">
+        <v>2020-02-12 07:46</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="str">
+        <v>新型冠状病毒正式命名为“COVID-19” 世卫组织解释命名原则</v>
+      </c>
+      <c r="B229">
+        <v>31773</v>
+      </c>
+      <c r="C229" t="str">
+        <v>2020-02-12 07:11</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="str">
+        <v>央视主播：复工做好本职工作，让经济有活力、为战“疫”添火力</v>
+      </c>
+      <c r="B230">
+        <v>2163</v>
+      </c>
+      <c r="C230" t="str">
+        <v>2020-02-12 04:45</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="str">
+        <v>催泪！湖北籍空姐通过广播哽咽致敬驰援家乡的福建医疗队</v>
+      </c>
+      <c r="B231">
+        <v>876010</v>
+      </c>
+      <c r="C231" t="str">
+        <v>2020-02-12 00:54</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="str">
+        <v>加油吧，中国少年！教师枯坐屋顶顶着大风开热点稳信号直播授课</v>
+      </c>
+      <c r="B232">
+        <v>11886</v>
+      </c>
+      <c r="C232" t="str">
+        <v>2020-02-12 00:39</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="str">
+        <v>辽宁葫芦岛一企业突发爆炸 已致2死3失联6伤</v>
+      </c>
+      <c r="B233">
+        <v>1999</v>
+      </c>
+      <c r="C233" t="str">
+        <v>2020-02-12 00:28</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="str">
+        <v>湖北省新闻发布会：最难治的是有基础疾病的高龄患者</v>
+      </c>
+      <c r="B234">
+        <v>29243</v>
+      </c>
+      <c r="C234" t="str">
+        <v>2020-02-11 22:51</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="str">
+        <v>湖南对口援助黄冈前方指挥部总指挥介绍新冠肺炎治疗手段</v>
+      </c>
+      <c r="B235">
+        <v>7430</v>
+      </c>
+      <c r="C235" t="str">
+        <v>2020-02-11 22:47</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="str">
+        <v>黄冈市委书记：黄冈N95口罩、防护服等紧缺 四渠道筹措</v>
+      </c>
+      <c r="B236">
+        <v>4735</v>
+      </c>
+      <c r="C236" t="str">
+        <v>2020-02-11 22:14</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="str">
+        <v>你家的扫帚今天立起来了吗？NASA立扫把挑战火爆朋友圈 然而真相是…</v>
+      </c>
+      <c r="B237">
+        <v>130944</v>
+      </c>
+      <c r="C237" t="str">
+        <v>2020-02-11 22:11</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="str">
+        <v>新冠肺炎救治：躯体治疗与心理治疗并重 中药在疾病早期介入成效明显</v>
+      </c>
+      <c r="B238">
+        <v>10291</v>
+      </c>
+      <c r="C238" t="str">
+        <v>2020-02-11 22:07</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="str">
+        <v>黄冈市委书记：村、社区排查1748.6万人次，发现发热病人13000人</v>
+      </c>
+      <c r="B239">
+        <v>203035</v>
+      </c>
+      <c r="C239" t="str">
+        <v>2020-02-11 21:46</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="str">
+        <v>黄冈市委书记：黄冈疫情前期存量全部检测完毕</v>
+      </c>
+      <c r="B240">
+        <v>23312</v>
+      </c>
+      <c r="C240" t="str">
+        <v>2020-02-11 21:44</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="str">
+        <v>中央赴湖北指导组：提高收治能力，宁可让床等人也不要让人等床</v>
+      </c>
+      <c r="B241">
+        <v>978625</v>
+      </c>
+      <c r="C241" t="str">
+        <v>2020-02-11 21:19</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="str">
+        <v>躺在ICU刷手机！他打破常人对ICU所想，被医护唤作“淡定哥”</v>
+      </c>
+      <c r="B242">
+        <v>46368</v>
+      </c>
+      <c r="C242" t="str">
+        <v>2020-02-11 20:42</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="str">
+        <v>致敬！7项措施关心防控一线医务人员</v>
+      </c>
+      <c r="B243">
+        <v>6024</v>
+      </c>
+      <c r="C243" t="str">
+        <v>2020-02-11 20:34</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="str">
+        <v>妈妈烧饭炉火未关，留女儿在家 消防破门一看：孩子上网课睡着了</v>
+      </c>
+      <c r="B244">
+        <v>5161</v>
+      </c>
+      <c r="C244" t="str">
+        <v>2020-02-11 20:09</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="str">
+        <v>连线：钟南山称峰值应在二月中下旬  拐点是否出现要看二次返程情况</v>
+      </c>
+      <c r="B245">
+        <v>1690355</v>
+      </c>
+      <c r="C245" t="str">
+        <v>2020-02-11 19:34</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="str">
+        <v>待腻了！萌娃们在家待着直呼“想出去玩” 各种神回复笑翻网友</v>
+      </c>
+      <c r="B246">
+        <v>75759</v>
+      </c>
+      <c r="C246" t="str">
+        <v>2020-02-11 18:20</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="str">
+        <v>女子不戴口罩掌掴、脚踢防疫执勤人员 叫嚣：你打我，我怀孕了</v>
+      </c>
+      <c r="B247">
+        <v>398317</v>
+      </c>
+      <c r="C247" t="str">
+        <v>2020-02-11 18:15</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="str">
+        <v>钟南山：全国疫情拐点无法预测，但峰值应在二月中下旬出现</v>
+      </c>
+      <c r="B248">
+        <v>5169563</v>
+      </c>
+      <c r="C248" t="str">
+        <v>2020-02-11 18:04</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="str">
+        <v>3秒钟隔空拥抱当团圆 浙江抗疫一线医生与丈夫的相聚让人泪目</v>
+      </c>
+      <c r="B249">
+        <v>58498</v>
+      </c>
+      <c r="C249" t="str">
+        <v>2020-02-11 17:46</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="str">
+        <v>国家卫健委：全国有144万乡村医生 56万乡村医生已开展网上学习</v>
+      </c>
+      <c r="B250">
+        <v>18394</v>
+      </c>
+      <c r="C250" t="str">
+        <v>2020-02-11 17:39</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="str">
+        <v>刚刚，武汉方舱医院首批治愈者出院 现场高呼：武汉加油</v>
+      </c>
+      <c r="B251">
+        <v>42670</v>
+      </c>
+      <c r="C251" t="str">
+        <v>2020-02-11 17:34</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="str">
+        <v>“我们要笑着面对一切！”病房内，护士病人同唱《我和我的祖国》</v>
+      </c>
+      <c r="B252">
+        <v>1176</v>
+      </c>
+      <c r="C252" t="str">
+        <v>2020-02-11 17:17</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="str">
+        <v>聚集性疫情是怎么发生的？如何防范？中国疾控中心专家回应</v>
+      </c>
+      <c r="B253">
+        <v>21505</v>
+      </c>
+      <c r="C253" t="str">
+        <v>2020-02-11 17:02</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="str">
+        <v>中国疾控中心专家：聚集性疫情83%是以家庭为单位</v>
+      </c>
+      <c r="B254">
+        <v>1508</v>
+      </c>
+      <c r="C254" t="str">
+        <v>2020-02-11 16:55</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="str">
+        <v>各地新冠肺炎患者出院标准不同？国家卫健委：全国一个标准</v>
+      </c>
+      <c r="B255">
+        <v>3616</v>
+      </c>
+      <c r="C255" t="str">
+        <v>2020-02-11 16:50</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="str">
+        <v>转存！出门一定要戴口罩！央视主播教你口罩这样省着用</v>
+      </c>
+      <c r="B256">
+        <v>18227</v>
+      </c>
+      <c r="C256" t="str">
+        <v>2020-02-11 16:44</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="str">
+        <v>上班路上如何做好防护？请牢记#28字通勤防疫口诀#</v>
+      </c>
+      <c r="B257">
+        <v>835564</v>
+      </c>
+      <c r="C257" t="str">
+        <v>2020-02-11 16:16</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="str">
+        <v>实拍武汉住宅小区严格执行封闭管理</v>
+      </c>
+      <c r="B258">
+        <v>71726</v>
+      </c>
+      <c r="C258" t="str">
+        <v>2020-02-11 16:04</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="str">
+        <v>四川多人聚众打牌被查 检讨发朋友圈集20个赞才能走！</v>
+      </c>
+      <c r="B259">
+        <v>15120</v>
+      </c>
+      <c r="C259" t="str">
+        <v>2020-02-11 15:56</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="str">
+        <v>硬核！奶奶“暴风雨式”教育乱串的老伴：再乱跑就给你脚杆打断</v>
+      </c>
+      <c r="B260">
+        <v>20196</v>
+      </c>
+      <c r="C260" t="str">
+        <v>2020-02-11 15:27</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="str">
+        <v>男子强闯防疫卡点，现场向民警叫嚣“杀头也不戴口罩”</v>
+      </c>
+      <c r="B261">
+        <v>68319</v>
+      </c>
+      <c r="C261" t="str">
+        <v>2020-02-11 15:09</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="str">
+        <v>没买到口罩送给民警，女孩就把陪伴12年的存钱罐给捐了</v>
+      </c>
+      <c r="B262">
+        <v>26603</v>
+      </c>
+      <c r="C262" t="str">
+        <v>2020-02-11 14:49</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="str">
+        <v>情侣撒狗粮被无人机连抓两次 社工隔空劝话：戴口罩也不影响的</v>
+      </c>
+      <c r="B263">
+        <v>3923587</v>
+      </c>
+      <c r="C263" t="str">
+        <v>2020-02-11 14:41</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="str">
+        <v>紧急扩散！陕西一高铁保洁员确诊新冠肺炎 曾搭乘这20趟高铁</v>
+      </c>
+      <c r="B264">
+        <v>32331</v>
+      </c>
+      <c r="C264" t="str">
+        <v>2020-02-11 14:08</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="str">
+        <v>世卫组织总干事谭德塞：感谢湖北人民，我的心一直与他们在一起</v>
+      </c>
+      <c r="B265">
+        <v>35599</v>
+      </c>
+      <c r="C265" t="str">
+        <v>2020-02-11 13:13</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="str">
+        <v>卫健委：全国疫情呈下降趋势 湖北以外地区新增确诊病例七连降</v>
+      </c>
+      <c r="B266">
+        <v>94786</v>
+      </c>
+      <c r="C266" t="str">
+        <v>2020-02-11 12:54</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="str">
+        <v>国家发改委：企业复工要为职工配发口罩等防护用品</v>
+      </c>
+      <c r="B267">
+        <v>124861</v>
+      </c>
+      <c r="C267" t="str">
+        <v>2020-02-11 12:35</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="str">
+        <v>地方设置门槛限制企业复工复产？发改委：此风不可长，将严格制止</v>
+      </c>
+      <c r="B268">
+        <v>152164</v>
+      </c>
+      <c r="C268" t="str">
+        <v>2020-02-11 12:16</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="str">
+        <v>交通运输部：截止2月18日春运结束 还将有1.6亿人返城返岗</v>
+      </c>
+      <c r="B269">
+        <v>200151</v>
+      </c>
+      <c r="C269" t="str">
+        <v>2020-02-11 12:06</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="str">
+        <v>复工后有员工确诊？国家卫健委：有发现，快隔离，有情况，快送医</v>
+      </c>
+      <c r="B270">
+        <v>76186</v>
+      </c>
+      <c r="C270" t="str">
+        <v>2020-02-11 12:01</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="str">
+        <v>发改委：严格杜绝填表抗疫等形式主义和官僚主义行为</v>
+      </c>
+      <c r="B271">
+        <v>99573</v>
+      </c>
+      <c r="C271" t="str">
+        <v>2020-02-11 11:21</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="str">
+        <v>国家发改委：全国口罩企业复工率已超76%，防控服企业复工率达77%</v>
+      </c>
+      <c r="B272">
+        <v>494954</v>
+      </c>
+      <c r="C272" t="str">
+        <v>2020-02-11 11:12</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="str">
+        <v>“哟，你比我还厉害嘞！”安阳城管队员大闹疫情卡点辱骂社工</v>
+      </c>
+      <c r="B273">
+        <v>13557</v>
+      </c>
+      <c r="C273" t="str">
+        <v>2020-02-11 10:55</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="str">
+        <v>温暖！为减少保洁员感染风险 武汉方舱医院患者主动搬运垃圾</v>
+      </c>
+      <c r="B274">
+        <v>49026</v>
+      </c>
+      <c r="C274" t="str">
+        <v>2020-02-11 10:19</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="str">
+        <v>安全又便捷！北京一馒头店自制“木滑梯”售卖食品 市民自发排队购买</v>
+      </c>
+      <c r="B275">
+        <v>40610</v>
+      </c>
+      <c r="C275" t="str">
+        <v>2020-02-11 10:06</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="str">
+        <v>电吹风能消毒让口罩重复用？专家手把手教你“复活”全过程</v>
+      </c>
+      <c r="B276">
+        <v>557321</v>
+      </c>
+      <c r="C276" t="str">
+        <v>2020-02-11 09:19</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="str">
+        <v>疫线医生夫妻科室相距不足百米却十多天没见 隔墙问候纸笔传情</v>
+      </c>
+      <c r="B277">
+        <v>255157</v>
+      </c>
+      <c r="C277" t="str">
+        <v>2020-02-11 08:55</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="str">
+        <v>居家隔离恐慌焦虑怎么办？心理专家：少刷新闻多看剧，保持运动</v>
+      </c>
+      <c r="B278">
+        <v>5492185</v>
+      </c>
+      <c r="C278" t="str">
+        <v>2020-02-11 08:24</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="str">
+        <v>画风清奇！从武汉撤离的俄罗斯人 在西伯利亚开了隔离“真人秀”</v>
+      </c>
+      <c r="B279">
+        <v>77921</v>
+      </c>
+      <c r="C279" t="str">
+        <v>2020-02-11 07:08</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="str">
+        <v>无人机硬核劝退又来了！别骑马出门了 “就是骑龙也不行！”</v>
+      </c>
+      <c r="B280">
+        <v>671706</v>
+      </c>
+      <c r="C280" t="str">
+        <v>2020-02-11 06:55</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="str">
+        <v>防疫硬核穿搭来了！复工第一天穿上这些“战袍” 瞬间安全感爆棚</v>
+      </c>
+      <c r="B281">
+        <v>31250</v>
+      </c>
+      <c r="C281" t="str">
+        <v>2020-02-11 06:44</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="str">
+        <v>央视主播：武汉，别怕！全国人民都在和你们并肩战斗！</v>
+      </c>
+      <c r="B282">
+        <v>3713</v>
+      </c>
+      <c r="C282" t="str">
+        <v>2020-02-10 23:56</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="str">
+        <v>雷神山医院院长：目前已接诊88人 预计17、18日实现接诊满员目标</v>
+      </c>
+      <c r="B283">
+        <v>11233</v>
+      </c>
+      <c r="C283" t="str">
+        <v>2020-02-10 23:40</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="str">
+        <v>金银潭医院院长答网友提问：一次性防护服消毒后不能再使用</v>
+      </c>
+      <c r="B284">
+        <v>94507</v>
+      </c>
+      <c r="C284" t="str">
+        <v>2020-02-10 22:40</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="str">
+        <v>济宁回应“保洁领口罩拍照后被收回”：之前已发放 公司要拍照取证</v>
+      </c>
+      <c r="B285">
+        <v>630066</v>
+      </c>
+      <c r="C285" t="str">
+        <v>2020-02-10 22:25</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="str">
+        <v>金银潭医院院长：医院1500余患者大多可顺利出院，市民不必过分恐慌</v>
+      </c>
+      <c r="B286">
+        <v>58932</v>
+      </c>
+      <c r="C286" t="str">
+        <v>2020-02-10 22:09</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="str">
+        <v>自信才是最大的免疫力！方舱医院内护士身穿防护服领跳广场舞</v>
+      </c>
+      <c r="B287">
+        <v>5218872</v>
+      </c>
+      <c r="C287" t="str">
+        <v>2020-02-10 22:07</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="str">
+        <v>武汉：1499名重症患者全部入院，11日拟将完成所有疑似患者检测清零</v>
+      </c>
+      <c r="B288">
+        <v>7622</v>
+      </c>
+      <c r="C288" t="str">
+        <v>2020-02-10 21:48</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="str">
+        <v>武汉市委书记：全市截至9日共排查1059万人，排查占比达99%</v>
+      </c>
+      <c r="B289">
+        <v>107992</v>
+      </c>
+      <c r="C289" t="str">
+        <v>2020-02-10 21:27</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="str">
+        <v>疫线民警家门外吃汤圆，看见女儿站在门口喊爸爸赶紧戴上了口罩</v>
+      </c>
+      <c r="B290">
+        <v>13175</v>
+      </c>
+      <c r="C290" t="str">
+        <v>2020-02-10 20:58</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="str">
+        <v>刑拘！女子因与他人纠纷故意向电梯按键吐口水，监控记录全过程</v>
+      </c>
+      <c r="B291">
+        <v>14188</v>
+      </c>
+      <c r="C291" t="str">
+        <v>2020-02-10 20:17</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="str">
+        <v>上课啦！武汉中小学今天正式“线上开课” 来看看和平时有啥不一样</v>
+      </c>
+      <c r="B292">
+        <v>59359</v>
+      </c>
+      <c r="C292" t="str">
+        <v>2020-02-10 19:42</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="str">
+        <v>解密！新冠病毒核酸检测，是这样做出来的！</v>
+      </c>
+      <c r="B293">
+        <v>372950</v>
+      </c>
+      <c r="C293" t="str">
+        <v>2020-02-10 19:42</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="str">
+        <v>致敬！消防员丈夫向援鄂抗“疫”妻子敬礼告别</v>
+      </c>
+      <c r="B294">
+        <v>61184</v>
+      </c>
+      <c r="C294" t="str">
+        <v>2020-02-10 19:40</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="str">
+        <v>北京市疾控中心：北京市共发生73起聚集性疫情 已有197人确诊</v>
+      </c>
+      <c r="B295">
+        <v>40700</v>
+      </c>
+      <c r="C295" t="str">
+        <v>2020-02-10 18:28</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="str">
+        <v>封闭社区管理后如何解决日常生活需求？民政部支招</v>
+      </c>
+      <c r="B296">
+        <v>17495</v>
+      </c>
+      <c r="C296" t="str">
+        <v>2020-02-10 17:51</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="str">
+        <v>群众网络买口罩捐赠医务人员被骗 嫌疑人被抓时正蒙头大睡</v>
+      </c>
+      <c r="B297">
+        <v>17559</v>
+      </c>
+      <c r="C297" t="str">
+        <v>2020-02-10 17:48</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="str">
+        <v>遇到身体不舒服就怀疑得了新冠肺炎？甚至开始服药？专家支招</v>
+      </c>
+      <c r="B298">
+        <v>94555</v>
+      </c>
+      <c r="C298" t="str">
+        <v>2020-02-10 17:38</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="str">
+        <v>民政部指责“往电梯按钮吐口水”行为：没有公德</v>
+      </c>
+      <c r="B299">
+        <v>175057</v>
+      </c>
+      <c r="C299" t="str">
+        <v>2020-02-10 17:31</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="str">
+        <v>小区封闭管理会不会推广到全国？民政部回应：因地制宜</v>
+      </c>
+      <c r="B300">
+        <v>61445</v>
+      </c>
+      <c r="C300" t="str">
+        <v>2020-02-10 17:07</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="str">
+        <v>非湖北返程人员是否需要隔离14天？民政部：可向社区了解</v>
+      </c>
+      <c r="B301">
+        <v>3533</v>
+      </c>
+      <c r="C301" t="str">
+        <v>2020-02-10 16:41</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="str">
+        <v>湖北两男子步行到湖南，称想坐火车回深圳上班 被铁警劝返</v>
+      </c>
+      <c r="B302">
+        <v>117355</v>
+      </c>
+      <c r="C302" t="str">
+        <v>2020-02-10 16:40</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="str">
+        <v>婚姻登记何时恢复？民政部：视疫情好转的情况逐步恢复登记</v>
+      </c>
+      <c r="B303">
+        <v>23644</v>
+      </c>
+      <c r="C303" t="str">
+        <v>2020-02-10 16:38</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="str">
+        <v>湖北襄阳：农机进城成消毒“神器” 360度无死角消毒</v>
+      </c>
+      <c r="B304">
+        <v>55426</v>
+      </c>
+      <c r="C304" t="str">
+        <v>2020-02-10 16:37</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="str">
+        <v>全国多地暂停婚姻登记 民政部：这是根据当地疫情情况作出的决定</v>
+      </c>
+      <c r="B305">
+        <v>9193</v>
+      </c>
+      <c r="C305" t="str">
+        <v>2020-02-10 16:30</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="str">
+        <v>民政部：疫情期间建议采取电话、视频方式探视养老机构老人</v>
+      </c>
+      <c r="B306">
+        <v>15130</v>
+      </c>
+      <c r="C306" t="str">
+        <v>2020-02-10 16:28</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="str">
+        <v>社区居民使用同一个体温计是否会造成交叉感染？民政部回应</v>
+      </c>
+      <c r="B307">
+        <v>1371</v>
+      </c>
+      <c r="C307" t="str">
+        <v>2020-02-10 16:14</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="str">
+        <v>河南一医院院长过卡点拒戴口罩，连说16句“我不戴”！被免职</v>
+      </c>
+      <c r="B308">
+        <v>5372</v>
+      </c>
+      <c r="C308" t="str">
+        <v>2020-02-10 15:44</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="str">
+        <v>国务院联防联控机制新闻发布会：全国治愈比例8.2% 明显上升</v>
+      </c>
+      <c r="B309">
+        <v>13522</v>
+      </c>
+      <c r="C309" t="str">
+        <v>2020-02-10 15:40</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="str">
+        <v>济宁回应“保洁领口罩拍照后被收回”：之前已发放 公司要拍照取证</v>
+      </c>
+      <c r="B310">
+        <v>13954</v>
+      </c>
+      <c r="C310" t="str">
+        <v>2020-02-10 15:33</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="str">
+        <v>上海疾控专家：现在说拐点到来为时过早，千万不能心存侥幸</v>
+      </c>
+      <c r="B311">
+        <v>3399</v>
+      </c>
+      <c r="C311" t="str">
+        <v>2020-02-10 15:33</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="str">
+        <v>继大妈领跳广场舞后，武汉方舱医院医患又打起了太极</v>
+      </c>
+      <c r="B312">
+        <v>3474</v>
+      </c>
+      <c r="C312" t="str">
+        <v>2020-02-10 15:31</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="str">
+        <v>湖北隔离病房内的感动！患者向所住医院捐款三万，感恩医护人员</v>
+      </c>
+      <c r="B313">
+        <v>41411</v>
+      </c>
+      <c r="C313" t="str">
+        <v>2020-02-10 14:37</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="str">
+        <v>不一样的课间操！河南全体中小学生居家在线做广播体操</v>
+      </c>
+      <c r="B314">
+        <v>11650</v>
+      </c>
+      <c r="C314" t="str">
+        <v>2020-02-10 14:27</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="str">
+        <v>警方无人机高空扫街，喊话劝离打麻将阿姨“戴口罩，马上散开”</v>
+      </c>
+      <c r="B315">
+        <v>106292</v>
+      </c>
+      <c r="C315" t="str">
+        <v>2020-02-10 14:21</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="str">
+        <v>一省包一市强援抵达！41架包机近6000人同天抵达武汉</v>
+      </c>
+      <c r="B316">
+        <v>696944</v>
+      </c>
+      <c r="C316" t="str">
+        <v>2020-02-10 13:12</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="str">
+        <v>青海玉树天空有“三个太阳” 气象专家释疑罕见“幻日”</v>
+      </c>
+      <c r="B317">
+        <v>45146</v>
+      </c>
+      <c r="C317" t="str">
+        <v>2020-02-10 12:15</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="str">
+        <v>“决胜时刻，We guide you home！”这段塔台对话让人泪目</v>
+      </c>
+      <c r="B318">
+        <v>404585</v>
+      </c>
+      <c r="C318" t="str">
+        <v>2020-02-10 11:47</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="str">
+        <v>“再问跟你急！”6旬夫妇为武汉捐款，民警追问姓名逼得他们要跳脚</v>
+      </c>
+      <c r="B319">
+        <v>73294</v>
+      </c>
+      <c r="C319" t="str">
+        <v>2020-02-10 11:31</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="str">
+        <v>阳台上玩耍的狗狗瞥了一眼楼下瞬间愣住 嘴里的小黄鸭突然不香了</v>
+      </c>
+      <c r="B320">
+        <v>589824</v>
+      </c>
+      <c r="C320" t="str">
+        <v>2020-02-10 11:24</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="str">
+        <v>抗疫一线女医生怕传染家人雨夜步行上班 丈夫凌晨默默用车灯护航</v>
+      </c>
+      <c r="B321">
+        <v>1571831</v>
+      </c>
+      <c r="C321" t="str">
+        <v>2020-02-10 10:59</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="str">
+        <v>女子自称医生拒戴口罩 呵斥检查人员：为什么要戴？没必要！</v>
+      </c>
+      <c r="B322">
+        <v>23195</v>
+      </c>
+      <c r="C322" t="str">
+        <v>2020-02-10 10:32</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="str">
+        <v>硬核防疫！警察飚四种语言喊话居民 ：少出门，no party！</v>
+      </c>
+      <c r="B323">
+        <v>57122</v>
+      </c>
+      <c r="C323" t="str">
+        <v>2020-02-10 08:40</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="str">
+        <v>医院副院长途经卡点拒戴口罩被停职：连说16个我不戴，还找局长告状</v>
+      </c>
+      <c r="B324">
+        <v>1497223</v>
+      </c>
+      <c r="C324" t="str">
+        <v>2020-02-10 08:38</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="str">
+        <v>好样的！宁夏8岁小孩把零花钱捐给武汉，民警敬礼致谢感动网友</v>
+      </c>
+      <c r="B325">
+        <v>72754</v>
+      </c>
+      <c r="C325" t="str">
+        <v>2020-02-10 06:56</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="str">
+        <v>武汉120调度员：封城后每天接上万个电话，有时数百单无车可派</v>
+      </c>
+      <c r="B326">
+        <v>109893</v>
+      </c>
+      <c r="C326" t="str">
+        <v>2020-02-10 06:44</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="str">
+        <v>服务员跨界当起了送货员 海霞赞“共享员工”新模式：很机智！</v>
+      </c>
+      <c r="B327">
+        <v>6486</v>
+      </c>
+      <c r="C327" t="str">
+        <v>2020-02-10 06:39</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="str">
+        <v>武汉协和首批确诊医护人员如何痊愈?主治医师解答</v>
+      </c>
+      <c r="B328">
+        <v>298645</v>
+      </c>
+      <c r="C328" t="str">
+        <v>2020-02-10 06:37</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C164"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C328"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>